<commit_message>
Updated Andrew's score on 1/31/22
</commit_message>
<xml_diff>
--- a/Wordle Tracking.xlsx
+++ b/Wordle Tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rriesenb\Personal\Wordle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{913DEE8B-5BE1-48B1-A65F-598E6DCA3B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F679EDAE-3432-436F-B23B-0B7835468805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F705EBF7-AD41-4B67-999F-6C40503692F5}"/>
   </bookViews>
@@ -523,7 +523,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
+      <selection pane="bottomLeft" activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1327,7 +1327,9 @@
         <f t="array" aca="1" ref="D41" ca="1">IF(_xlfn.XLOOKUP($B41,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B41,wordle_ids,wordles))</f>
         <v>LIGHT</v>
       </c>
-      <c r="E41" s="10"/>
+      <c r="E41" s="10">
+        <v>5</v>
+      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2">

</xml_diff>

<commit_message>
Updated everyone but Phil for 2/2/22
</commit_message>
<xml_diff>
--- a/Wordle Tracking.xlsx
+++ b/Wordle Tracking.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rriesenb\Personal\Wordle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F679EDAE-3432-436F-B23B-0B7835468805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E43A8D-7AB2-46E4-8F36-680B941F8254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F705EBF7-AD41-4B67-999F-6C40503692F5}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -128,6 +128,12 @@
   </si>
   <si>
     <t>COULD</t>
+  </si>
+  <si>
+    <t>THOSE</t>
+  </si>
+  <si>
+    <t>MOIST</t>
   </si>
 </sst>
 </file>
@@ -522,8 +528,8 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E42" sqref="E42"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -879,7 +885,7 @@
         <v>44224</v>
       </c>
       <c r="B20" s="6">
-        <f t="shared" ref="B20:B43" si="0">B14+1</f>
+        <f t="shared" ref="B20:B55" si="0">B14+1</f>
         <v>223</v>
       </c>
       <c r="C20" s="2" t="str">
@@ -896,7 +902,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <f t="shared" ref="A21:A42" si="1">A15+1</f>
+        <f t="shared" ref="A21:A55" si="1">A15+1</f>
         <v>44224</v>
       </c>
       <c r="B21" s="6">
@@ -904,7 +910,7 @@
         <v>223</v>
       </c>
       <c r="C21" s="2" t="str">
-        <f t="shared" ref="C21:C42" si="2">C15</f>
+        <f t="shared" ref="C21:C55" si="2">C15</f>
         <v>Erik</v>
       </c>
       <c r="D21" t="str" cm="1">
@@ -1374,66 +1380,280 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E44" s="10"/>
+      <c r="A44" s="2">
+        <f t="shared" si="1"/>
+        <v>44228</v>
+      </c>
+      <c r="B44" s="6">
+        <f t="shared" si="0"/>
+        <v>227</v>
+      </c>
+      <c r="C44" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Phil</v>
+      </c>
+      <c r="D44" t="str" cm="1">
+        <f t="array" aca="1" ref="D44" ca="1">IF(_xlfn.XLOOKUP($B44,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B44,wordle_ids,wordles))</f>
+        <v>THOSE</v>
+      </c>
+      <c r="E44" s="10">
+        <v>2</v>
+      </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E45" s="10"/>
+      <c r="A45" s="2">
+        <f t="shared" si="1"/>
+        <v>44228</v>
+      </c>
+      <c r="B45" s="6">
+        <f t="shared" si="0"/>
+        <v>227</v>
+      </c>
+      <c r="C45" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Erik</v>
+      </c>
+      <c r="D45" t="str" cm="1">
+        <f t="array" aca="1" ref="D45" ca="1">IF(_xlfn.XLOOKUP($B45,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B45,wordle_ids,wordles))</f>
+        <v>THOSE</v>
+      </c>
+      <c r="E45" s="10">
+        <v>2</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E46" s="10"/>
+      <c r="A46" s="2">
+        <f t="shared" si="1"/>
+        <v>44228</v>
+      </c>
+      <c r="B46" s="6">
+        <f t="shared" si="0"/>
+        <v>227</v>
+      </c>
+      <c r="C46" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>RoBert</v>
+      </c>
+      <c r="D46" t="str" cm="1">
+        <f t="array" aca="1" ref="D46" ca="1">IF(_xlfn.XLOOKUP($B46,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B46,wordle_ids,wordles))</f>
+        <v>THOSE</v>
+      </c>
+      <c r="E46" s="10">
+        <v>3</v>
+      </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E47" s="10"/>
+      <c r="A47" s="2">
+        <f t="shared" si="1"/>
+        <v>44228</v>
+      </c>
+      <c r="B47" s="6">
+        <f t="shared" si="0"/>
+        <v>227</v>
+      </c>
+      <c r="C47" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Andrew</v>
+      </c>
+      <c r="D47" t="str" cm="1">
+        <f t="array" aca="1" ref="D47" ca="1">IF(_xlfn.XLOOKUP($B47,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B47,wordle_ids,wordles))</f>
+        <v>THOSE</v>
+      </c>
+      <c r="E47" s="10">
+        <v>4</v>
+      </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E48" s="10"/>
-    </row>
-    <row r="49" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E49" s="10"/>
-    </row>
-    <row r="50" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <f t="shared" si="1"/>
+        <v>44228</v>
+      </c>
+      <c r="B48" s="6">
+        <f t="shared" si="0"/>
+        <v>227</v>
+      </c>
+      <c r="C48" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Yoyo</v>
+      </c>
+      <c r="D48" t="str" cm="1">
+        <f t="array" aca="1" ref="D48" ca="1">IF(_xlfn.XLOOKUP($B48,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B48,wordle_ids,wordles))</f>
+        <v>THOSE</v>
+      </c>
+      <c r="E48" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
+        <f t="shared" si="1"/>
+        <v>44228</v>
+      </c>
+      <c r="B49" s="6">
+        <f t="shared" si="0"/>
+        <v>227</v>
+      </c>
+      <c r="C49" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Henry</v>
+      </c>
+      <c r="D49" t="str" cm="1">
+        <f t="array" aca="1" ref="D49" ca="1">IF(_xlfn.XLOOKUP($B49,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B49,wordle_ids,wordles))</f>
+        <v>THOSE</v>
+      </c>
+      <c r="E49" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <f t="shared" si="1"/>
+        <v>44229</v>
+      </c>
+      <c r="B50" s="6">
+        <f t="shared" si="0"/>
+        <v>228</v>
+      </c>
+      <c r="C50" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Phil</v>
+      </c>
+      <c r="D50" t="str" cm="1">
+        <f t="array" aca="1" ref="D50" ca="1">IF(_xlfn.XLOOKUP($B50,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B50,wordle_ids,wordles))</f>
+        <v>MOIST</v>
+      </c>
       <c r="E50" s="10"/>
     </row>
-    <row r="51" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E51" s="10"/>
-    </row>
-    <row r="52" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E52" s="10"/>
-    </row>
-    <row r="53" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E53" s="10"/>
-    </row>
-    <row r="54" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E54" s="10"/>
-    </row>
-    <row r="55" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E55" s="10"/>
-    </row>
-    <row r="56" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
+        <f t="shared" si="1"/>
+        <v>44229</v>
+      </c>
+      <c r="B51" s="6">
+        <f t="shared" si="0"/>
+        <v>228</v>
+      </c>
+      <c r="C51" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Erik</v>
+      </c>
+      <c r="D51" t="str" cm="1">
+        <f t="array" aca="1" ref="D51" ca="1">IF(_xlfn.XLOOKUP($B51,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B51,wordle_ids,wordles))</f>
+        <v>MOIST</v>
+      </c>
+      <c r="E51" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
+        <f t="shared" si="1"/>
+        <v>44229</v>
+      </c>
+      <c r="B52" s="6">
+        <f t="shared" si="0"/>
+        <v>228</v>
+      </c>
+      <c r="C52" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>RoBert</v>
+      </c>
+      <c r="D52" t="str" cm="1">
+        <f t="array" aca="1" ref="D52" ca="1">IF(_xlfn.XLOOKUP($B52,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B52,wordle_ids,wordles))</f>
+        <v>MOIST</v>
+      </c>
+      <c r="E52" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
+        <f t="shared" si="1"/>
+        <v>44229</v>
+      </c>
+      <c r="B53" s="6">
+        <f t="shared" si="0"/>
+        <v>228</v>
+      </c>
+      <c r="C53" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Andrew</v>
+      </c>
+      <c r="D53" t="str" cm="1">
+        <f t="array" aca="1" ref="D53" ca="1">IF(_xlfn.XLOOKUP($B53,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B53,wordle_ids,wordles))</f>
+        <v>MOIST</v>
+      </c>
+      <c r="E53" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
+        <f t="shared" si="1"/>
+        <v>44229</v>
+      </c>
+      <c r="B54" s="6">
+        <f t="shared" si="0"/>
+        <v>228</v>
+      </c>
+      <c r="C54" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Yoyo</v>
+      </c>
+      <c r="D54" t="str" cm="1">
+        <f t="array" aca="1" ref="D54" ca="1">IF(_xlfn.XLOOKUP($B54,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B54,wordle_ids,wordles))</f>
+        <v>MOIST</v>
+      </c>
+      <c r="E54" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
+        <f t="shared" si="1"/>
+        <v>44229</v>
+      </c>
+      <c r="B55" s="6">
+        <f t="shared" si="0"/>
+        <v>228</v>
+      </c>
+      <c r="C55" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Henry</v>
+      </c>
+      <c r="D55" t="str" cm="1">
+        <f t="array" aca="1" ref="D55" ca="1">IF(_xlfn.XLOOKUP($B55,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B55,wordle_ids,wordles))</f>
+        <v>MOIST</v>
+      </c>
+      <c r="E55" s="10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E56" s="10"/>
     </row>
-    <row r="57" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E57" s="10"/>
     </row>
-    <row r="58" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E58" s="10"/>
     </row>
-    <row r="59" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E59" s="10"/>
     </row>
-    <row r="60" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E60" s="10"/>
     </row>
-    <row r="61" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E61" s="10"/>
     </row>
-    <row r="62" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E62" s="10"/>
     </row>
-    <row r="63" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E63" s="10"/>
     </row>
-    <row r="64" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E64" s="10"/>
     </row>
     <row r="65" spans="5:5" x14ac:dyDescent="0.25">
@@ -1944,11 +2164,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0627B16-E6A6-4FDA-A605-D8A29593EF93}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1984,7 +2204,7 @@
         <v>44585</v>
       </c>
       <c r="B3" s="6">
-        <f t="shared" ref="B3:B10" si="0">B2+1</f>
+        <f t="shared" ref="B3:B12" si="0">B2+1</f>
         <v>219</v>
       </c>
       <c r="C3" s="9" t="s">
@@ -1993,7 +2213,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <f t="shared" ref="A4:A10" si="1">A3+1</f>
+        <f t="shared" ref="A4:A12" si="1">A3+1</f>
         <v>44586</v>
       </c>
       <c r="B4" s="6">
@@ -2080,6 +2300,32 @@
       </c>
       <c r="C10" s="9" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <f t="shared" si="1"/>
+        <v>44593</v>
+      </c>
+      <c r="B11" s="6">
+        <f t="shared" si="0"/>
+        <v>227</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <f t="shared" si="1"/>
+        <v>44594</v>
+      </c>
+      <c r="B12" s="6">
+        <f t="shared" si="0"/>
+        <v>228</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Partial update for 2/3/22
</commit_message>
<xml_diff>
--- a/Wordle Tracking.xlsx
+++ b/Wordle Tracking.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rriesenb\Personal\Wordle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E43A8D-7AB2-46E4-8F36-680B941F8254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25AA6F3B-6F26-4350-B847-71B90D30CC5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F705EBF7-AD41-4B67-999F-6C40503692F5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F705EBF7-AD41-4B67-999F-6C40503692F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
     <sheet name="Words" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Results!$A$1:$E$55</definedName>
     <definedName name="wordle_dates">OFFSET(Words!$A$2,,,COUNTA(Words!$A:$A)-1)</definedName>
     <definedName name="wordle_ids">OFFSET(Words!$B$2,,,COUNTA(Words!$B:$B)-1)</definedName>
     <definedName name="wordles">OFFSET(Words!$C$2,,,COUNTA(Words!$B:$B)-1)</definedName>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
   <si>
     <t>Date</t>
   </si>
@@ -134,6 +135,9 @@
   </si>
   <si>
     <t>MOIST</t>
+  </si>
+  <si>
+    <t>SHARD</t>
   </si>
 </sst>
 </file>
@@ -528,8 +532,8 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E51" sqref="E51"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,7 +889,7 @@
         <v>44224</v>
       </c>
       <c r="B20" s="6">
-        <f t="shared" ref="B20:B55" si="0">B14+1</f>
+        <f t="shared" ref="B20:B61" si="0">B14+1</f>
         <v>223</v>
       </c>
       <c r="C20" s="2" t="str">
@@ -902,7 +906,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <f t="shared" ref="A21:A55" si="1">A15+1</f>
+        <f t="shared" ref="A21:A61" si="1">A15+1</f>
         <v>44224</v>
       </c>
       <c r="B21" s="6">
@@ -910,7 +914,7 @@
         <v>223</v>
       </c>
       <c r="C21" s="2" t="str">
-        <f t="shared" ref="C21:C55" si="2">C15</f>
+        <f t="shared" ref="C21:C61" si="2">C15</f>
         <v>Erik</v>
       </c>
       <c r="D21" t="str" cm="1">
@@ -1522,7 +1526,9 @@
         <f t="array" aca="1" ref="D50" ca="1">IF(_xlfn.XLOOKUP($B50,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B50,wordle_ids,wordles))</f>
         <v>MOIST</v>
       </c>
-      <c r="E50" s="10"/>
+      <c r="E50" s="10">
+        <v>3</v>
+      </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
@@ -1630,22 +1636,126 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="2">
+        <f t="shared" si="1"/>
+        <v>44230</v>
+      </c>
+      <c r="B56" s="6">
+        <f t="shared" si="0"/>
+        <v>229</v>
+      </c>
+      <c r="C56" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Phil</v>
+      </c>
+      <c r="D56" t="str" cm="1">
+        <f t="array" aca="1" ref="D56" ca="1">IF(_xlfn.XLOOKUP($B56,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B56,wordle_ids,wordles))</f>
+        <v>SHARD</v>
+      </c>
       <c r="E56" s="10"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E57" s="10"/>
+      <c r="A57" s="2">
+        <f t="shared" si="1"/>
+        <v>44230</v>
+      </c>
+      <c r="B57" s="6">
+        <f t="shared" si="0"/>
+        <v>229</v>
+      </c>
+      <c r="C57" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Erik</v>
+      </c>
+      <c r="D57" t="str" cm="1">
+        <f t="array" aca="1" ref="D57" ca="1">IF(_xlfn.XLOOKUP($B57,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B57,wordle_ids,wordles))</f>
+        <v>SHARD</v>
+      </c>
+      <c r="E57" s="10">
+        <v>5</v>
+      </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E58" s="10"/>
+      <c r="A58" s="2">
+        <f t="shared" si="1"/>
+        <v>44230</v>
+      </c>
+      <c r="B58" s="6">
+        <f t="shared" si="0"/>
+        <v>229</v>
+      </c>
+      <c r="C58" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>RoBert</v>
+      </c>
+      <c r="D58" t="str" cm="1">
+        <f t="array" aca="1" ref="D58" ca="1">IF(_xlfn.XLOOKUP($B58,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B58,wordle_ids,wordles))</f>
+        <v>SHARD</v>
+      </c>
+      <c r="E58" s="10">
+        <v>5</v>
+      </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E59" s="10"/>
+      <c r="A59" s="2">
+        <f t="shared" si="1"/>
+        <v>44230</v>
+      </c>
+      <c r="B59" s="6">
+        <f t="shared" si="0"/>
+        <v>229</v>
+      </c>
+      <c r="C59" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Andrew</v>
+      </c>
+      <c r="D59" t="str" cm="1">
+        <f t="array" aca="1" ref="D59" ca="1">IF(_xlfn.XLOOKUP($B59,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B59,wordle_ids,wordles))</f>
+        <v>SHARD</v>
+      </c>
+      <c r="E59" s="10">
+        <v>4</v>
+      </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="2">
+        <f t="shared" si="1"/>
+        <v>44230</v>
+      </c>
+      <c r="B60" s="6">
+        <f t="shared" si="0"/>
+        <v>229</v>
+      </c>
+      <c r="C60" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Yoyo</v>
+      </c>
+      <c r="D60" t="str" cm="1">
+        <f t="array" aca="1" ref="D60" ca="1">IF(_xlfn.XLOOKUP($B60,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B60,wordle_ids,wordles))</f>
+        <v>SHARD</v>
+      </c>
       <c r="E60" s="10"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E61" s="10"/>
+      <c r="A61" s="2">
+        <f t="shared" si="1"/>
+        <v>44230</v>
+      </c>
+      <c r="B61" s="6">
+        <f t="shared" si="0"/>
+        <v>229</v>
+      </c>
+      <c r="C61" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Henry</v>
+      </c>
+      <c r="D61" t="str" cm="1">
+        <f t="array" aca="1" ref="D61" ca="1">IF(_xlfn.XLOOKUP($B61,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B61,wordle_ids,wordles))</f>
+        <v>SHARD</v>
+      </c>
+      <c r="E61" s="10">
+        <v>4</v>
+      </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E62" s="10"/>
@@ -2158,17 +2268,18 @@
       <c r="A1048576" s="2"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E55" xr:uid="{2D001387-04E3-4955-8CAF-0DBBBF22CEAF}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0627B16-E6A6-4FDA-A605-D8A29593EF93}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2204,7 +2315,7 @@
         <v>44585</v>
       </c>
       <c r="B3" s="6">
-        <f t="shared" ref="B3:B12" si="0">B2+1</f>
+        <f t="shared" ref="B3:B13" si="0">B2+1</f>
         <v>219</v>
       </c>
       <c r="C3" s="9" t="s">
@@ -2213,7 +2324,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <f t="shared" ref="A4:A12" si="1">A3+1</f>
+        <f t="shared" ref="A4:A13" si="1">A3+1</f>
         <v>44586</v>
       </c>
       <c r="B4" s="6">
@@ -2326,6 +2437,19 @@
       </c>
       <c r="C12" s="9" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <f t="shared" si="1"/>
+        <v>44595</v>
+      </c>
+      <c r="B13" s="6">
+        <f t="shared" si="0"/>
+        <v>229</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added in data for 2/4/22.
</commit_message>
<xml_diff>
--- a/Wordle Tracking.xlsx
+++ b/Wordle Tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rriesenb\Personal\Wordle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8450E441-E18A-4EDC-8C2F-8505B4DB1BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA088329-2713-4B65-AC8E-D847AE9A0D39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F705EBF7-AD41-4B67-999F-6C40503692F5}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
   <si>
     <t>Date</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>SHARD</t>
+  </si>
+  <si>
+    <t>PLEAT</t>
   </si>
 </sst>
 </file>
@@ -532,8 +535,8 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E58" sqref="E58"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -889,7 +892,7 @@
         <v>44224</v>
       </c>
       <c r="B20" s="6">
-        <f t="shared" ref="B20:B61" si="0">B14+1</f>
+        <f t="shared" ref="B20:B71" si="0">B14+1</f>
         <v>223</v>
       </c>
       <c r="C20" s="2" t="str">
@@ -906,7 +909,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <f t="shared" ref="A21:A61" si="1">A15+1</f>
+        <f t="shared" ref="A21:A71" si="1">A15+1</f>
         <v>44224</v>
       </c>
       <c r="B21" s="6">
@@ -914,7 +917,7 @@
         <v>223</v>
       </c>
       <c r="C21" s="2" t="str">
-        <f t="shared" ref="C21:C61" si="2">C15</f>
+        <f t="shared" ref="C21:C71" si="2">C15</f>
         <v>Erik</v>
       </c>
       <c r="D21" t="str" cm="1">
@@ -1762,60 +1765,180 @@
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E62" s="10"/>
+      <c r="A62" s="2">
+        <f t="shared" si="1"/>
+        <v>44231</v>
+      </c>
+      <c r="B62" s="6">
+        <f t="shared" si="0"/>
+        <v>230</v>
+      </c>
+      <c r="C62" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Phil</v>
+      </c>
+      <c r="D62" t="str" cm="1">
+        <f t="array" aca="1" ref="D62" ca="1">IF(_xlfn.XLOOKUP($B62,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B62,wordle_ids,wordles))</f>
+        <v>PLEAT</v>
+      </c>
+      <c r="E62" s="10">
+        <v>6</v>
+      </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E63" s="10"/>
+      <c r="A63" s="2">
+        <f t="shared" si="1"/>
+        <v>44231</v>
+      </c>
+      <c r="B63" s="6">
+        <f t="shared" si="0"/>
+        <v>230</v>
+      </c>
+      <c r="C63" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Erik</v>
+      </c>
+      <c r="D63" t="str" cm="1">
+        <f t="array" aca="1" ref="D63" ca="1">IF(_xlfn.XLOOKUP($B63,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B63,wordle_ids,wordles))</f>
+        <v>PLEAT</v>
+      </c>
+      <c r="E63" s="10">
+        <v>5</v>
+      </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E64" s="10"/>
-    </row>
-    <row r="65" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E65" s="10"/>
-    </row>
-    <row r="66" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E66" s="10"/>
-    </row>
-    <row r="67" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E67" s="10"/>
-    </row>
-    <row r="68" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="2">
+        <f t="shared" si="1"/>
+        <v>44231</v>
+      </c>
+      <c r="B64" s="6">
+        <f t="shared" si="0"/>
+        <v>230</v>
+      </c>
+      <c r="C64" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>RoBert</v>
+      </c>
+      <c r="D64" t="str" cm="1">
+        <f t="array" aca="1" ref="D64" ca="1">IF(_xlfn.XLOOKUP($B64,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B64,wordle_ids,wordles))</f>
+        <v>PLEAT</v>
+      </c>
+      <c r="E64" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="2">
+        <f t="shared" si="1"/>
+        <v>44231</v>
+      </c>
+      <c r="B65" s="6">
+        <f t="shared" si="0"/>
+        <v>230</v>
+      </c>
+      <c r="C65" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Andrew</v>
+      </c>
+      <c r="D65" t="str" cm="1">
+        <f t="array" aca="1" ref="D65" ca="1">IF(_xlfn.XLOOKUP($B65,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B65,wordle_ids,wordles))</f>
+        <v>PLEAT</v>
+      </c>
+      <c r="E65" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="2">
+        <f t="shared" si="1"/>
+        <v>44231</v>
+      </c>
+      <c r="B66" s="6">
+        <f t="shared" si="0"/>
+        <v>230</v>
+      </c>
+      <c r="C66" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Yoyo</v>
+      </c>
+      <c r="D66" t="str" cm="1">
+        <f t="array" aca="1" ref="D66" ca="1">IF(_xlfn.XLOOKUP($B66,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B66,wordle_ids,wordles))</f>
+        <v>PLEAT</v>
+      </c>
+      <c r="E66" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="2">
+        <f t="shared" si="1"/>
+        <v>44231</v>
+      </c>
+      <c r="B67" s="6">
+        <f t="shared" si="0"/>
+        <v>230</v>
+      </c>
+      <c r="C67" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Henry</v>
+      </c>
+      <c r="D67" t="str" cm="1">
+        <f t="array" aca="1" ref="D67" ca="1">IF(_xlfn.XLOOKUP($B67,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B67,wordle_ids,wordles))</f>
+        <v>PLEAT</v>
+      </c>
+      <c r="E67" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="2"/>
+      <c r="B68" s="6"/>
+      <c r="C68" s="2"/>
       <c r="E68" s="10"/>
     </row>
-    <row r="69" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="2"/>
+      <c r="B69" s="6"/>
+      <c r="C69" s="2"/>
       <c r="E69" s="10"/>
     </row>
-    <row r="70" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="2"/>
+      <c r="B70" s="6"/>
+      <c r="C70" s="2"/>
       <c r="E70" s="10"/>
     </row>
-    <row r="71" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="2"/>
+      <c r="B71" s="6"/>
+      <c r="C71" s="2"/>
       <c r="E71" s="10"/>
     </row>
-    <row r="72" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E72" s="10"/>
     </row>
-    <row r="73" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E73" s="10"/>
     </row>
-    <row r="74" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E74" s="10"/>
     </row>
-    <row r="75" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E75" s="10"/>
     </row>
-    <row r="76" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E76" s="10"/>
     </row>
-    <row r="77" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E77" s="10"/>
     </row>
-    <row r="78" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E78" s="10"/>
     </row>
-    <row r="79" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E79" s="10"/>
     </row>
-    <row r="80" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E80" s="10"/>
     </row>
     <row r="81" spans="5:5" x14ac:dyDescent="0.25">
@@ -2279,11 +2402,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0627B16-E6A6-4FDA-A605-D8A29593EF93}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2319,7 +2442,7 @@
         <v>44585</v>
       </c>
       <c r="B3" s="6">
-        <f t="shared" ref="B3:B13" si="0">B2+1</f>
+        <f t="shared" ref="B3:B14" si="0">B2+1</f>
         <v>219</v>
       </c>
       <c r="C3" s="9" t="s">
@@ -2328,7 +2451,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <f t="shared" ref="A4:A13" si="1">A3+1</f>
+        <f t="shared" ref="A4:A14" si="1">A3+1</f>
         <v>44586</v>
       </c>
       <c r="B4" s="6">
@@ -2454,6 +2577,19 @@
       </c>
       <c r="C13" s="9" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <f t="shared" si="1"/>
+        <v>44596</v>
+      </c>
+      <c r="B14" s="6">
+        <f t="shared" si="0"/>
+        <v>230</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Initial version up and running. Still need to add more charts to player page & create an ICW vs BFF's page
</commit_message>
<xml_diff>
--- a/Wordle Tracking.xlsx
+++ b/Wordle Tracking.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rriesenb\Personal\Wordle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riese\WordleTracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8450E441-E18A-4EDC-8C2F-8505B4DB1BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{305507D3-4739-43AC-99BC-493AE25F2409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F705EBF7-AD41-4B67-999F-6C40503692F5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F705EBF7-AD41-4B67-999F-6C40503692F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
     <sheet name="Words" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Results!$A$1:$E$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Results!$A$1:$E$67</definedName>
     <definedName name="wordle_dates">OFFSET(Words!$A$2,,,COUNTA(Words!$A:$A)-1)</definedName>
     <definedName name="wordle_ids">OFFSET(Words!$B$2,,,COUNTA(Words!$B:$B)-1)</definedName>
     <definedName name="wordles">OFFSET(Words!$C$2,,,COUNTA(Words!$B:$B)-1)</definedName>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -138,6 +138,15 @@
   </si>
   <si>
     <t>SHARD</t>
+  </si>
+  <si>
+    <t>SKILL</t>
+  </si>
+  <si>
+    <t>ALOFT</t>
+  </si>
+  <si>
+    <t>PLEAT</t>
   </si>
 </sst>
 </file>
@@ -529,11 +538,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D001387-04E3-4955-8CAF-0DBBBF22CEAF}">
-  <dimension ref="A1:E1048576"/>
+  <dimension ref="A1:E242"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E58" sqref="E58"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,290 +624,308 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>44220</v>
+        <v>44219</v>
       </c>
       <c r="B5" s="4">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D5" t="str" cm="1">
         <f t="array" aca="1" ref="D5" ca="1">IF(_xlfn.XLOOKUP($B5,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B5,wordle_ids,wordles))</f>
-        <v>KNOLL</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>18</v>
-      </c>
+        <v>CRIMP</v>
+      </c>
+      <c r="E5" s="10"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
-        <v>44220</v>
+        <v>44219</v>
       </c>
       <c r="B6" s="4">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D6" t="str" cm="1">
         <f t="array" aca="1" ref="D6" ca="1">IF(_xlfn.XLOOKUP($B6,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B6,wordle_ids,wordles))</f>
-        <v>KNOLL</v>
-      </c>
-      <c r="E6" s="10">
-        <v>5</v>
-      </c>
+        <v>CRIMP</v>
+      </c>
+      <c r="E6" s="10"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
-        <v>44220</v>
+        <v>44219</v>
       </c>
       <c r="B7" s="4">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D7" t="str" cm="1">
         <f t="array" aca="1" ref="D7" ca="1">IF(_xlfn.XLOOKUP($B7,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B7,wordle_ids,wordles))</f>
-        <v>KNOLL</v>
-      </c>
-      <c r="E7" s="10">
-        <v>5</v>
-      </c>
+        <v>CRIMP</v>
+      </c>
+      <c r="E7" s="10"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>44221</v>
-      </c>
-      <c r="B8" s="4">
-        <v>220</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>5</v>
+      <c r="A8" s="2">
+        <f t="shared" ref="A8:A31" si="0">A2+1</f>
+        <v>44220</v>
+      </c>
+      <c r="B8" s="6">
+        <f t="shared" ref="B8:B31" si="1">B2+1</f>
+        <v>219</v>
+      </c>
+      <c r="C8" s="2" t="str">
+        <f>C2</f>
+        <v>Phil</v>
       </c>
       <c r="D8" t="str" cm="1">
         <f t="array" aca="1" ref="D8" ca="1">IF(_xlfn.XLOOKUP($B8,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B8,wordle_ids,wordles))</f>
-        <v>SUGAR</v>
-      </c>
-      <c r="E8" s="10">
-        <v>4</v>
+        <v>KNOLL</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>44221</v>
-      </c>
-      <c r="B9" s="4">
-        <v>220</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>6</v>
+      <c r="A9" s="2">
+        <f t="shared" si="0"/>
+        <v>44220</v>
+      </c>
+      <c r="B9" s="6">
+        <f t="shared" si="1"/>
+        <v>219</v>
+      </c>
+      <c r="C9" s="2" t="str">
+        <f t="shared" ref="C9:C31" si="2">C3</f>
+        <v>Erik</v>
       </c>
       <c r="D9" t="str" cm="1">
         <f t="array" aca="1" ref="D9" ca="1">IF(_xlfn.XLOOKUP($B9,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B9,wordle_ids,wordles))</f>
-        <v>SUGAR</v>
+        <v>KNOLL</v>
       </c>
       <c r="E9" s="10">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>44221</v>
-      </c>
-      <c r="B10" s="4">
-        <v>220</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>7</v>
+      <c r="A10" s="2">
+        <f t="shared" si="0"/>
+        <v>44220</v>
+      </c>
+      <c r="B10" s="6">
+        <f t="shared" si="1"/>
+        <v>219</v>
+      </c>
+      <c r="C10" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>RoBert</v>
       </c>
       <c r="D10" t="str" cm="1">
         <f t="array" aca="1" ref="D10" ca="1">IF(_xlfn.XLOOKUP($B10,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B10,wordle_ids,wordles))</f>
-        <v>SUGAR</v>
+        <v>KNOLL</v>
       </c>
       <c r="E10" s="10">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>44222</v>
-      </c>
-      <c r="B11" s="4">
-        <v>221</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>5</v>
+      <c r="A11" s="2">
+        <f t="shared" si="0"/>
+        <v>44220</v>
+      </c>
+      <c r="B11" s="6">
+        <f t="shared" si="1"/>
+        <v>219</v>
+      </c>
+      <c r="C11" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Andrew</v>
       </c>
       <c r="D11" t="str" cm="1">
         <f t="array" aca="1" ref="D11" ca="1">IF(_xlfn.XLOOKUP($B11,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B11,wordle_ids,wordles))</f>
-        <v>WHACK</v>
-      </c>
-      <c r="E11" s="10">
-        <v>4</v>
-      </c>
+        <v>KNOLL</v>
+      </c>
+      <c r="E11" s="10"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>44222</v>
-      </c>
-      <c r="B12" s="4">
-        <v>221</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>6</v>
+      <c r="A12" s="2">
+        <f t="shared" si="0"/>
+        <v>44220</v>
+      </c>
+      <c r="B12" s="6">
+        <f t="shared" si="1"/>
+        <v>219</v>
+      </c>
+      <c r="C12" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Yoyo</v>
       </c>
       <c r="D12" t="str" cm="1">
         <f t="array" aca="1" ref="D12" ca="1">IF(_xlfn.XLOOKUP($B12,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B12,wordle_ids,wordles))</f>
-        <v>WHACK</v>
-      </c>
-      <c r="E12" s="10">
-        <v>5</v>
-      </c>
+        <v>KNOLL</v>
+      </c>
+      <c r="E12" s="10"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
-        <v>44222</v>
-      </c>
-      <c r="B13" s="4">
-        <v>221</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>7</v>
+      <c r="A13" s="2">
+        <f t="shared" si="0"/>
+        <v>44220</v>
+      </c>
+      <c r="B13" s="6">
+        <f t="shared" si="1"/>
+        <v>219</v>
+      </c>
+      <c r="C13" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Henry</v>
       </c>
       <c r="D13" t="str" cm="1">
         <f t="array" aca="1" ref="D13" ca="1">IF(_xlfn.XLOOKUP($B13,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B13,wordle_ids,wordles))</f>
-        <v>WHACK</v>
-      </c>
-      <c r="E13" s="10">
-        <v>4</v>
-      </c>
+        <v>KNOLL</v>
+      </c>
+      <c r="E13" s="10"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
-        <v>44223</v>
-      </c>
-      <c r="B14" s="4">
-        <v>222</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>5</v>
+      <c r="A14" s="2">
+        <f t="shared" si="0"/>
+        <v>44221</v>
+      </c>
+      <c r="B14" s="6">
+        <f t="shared" si="1"/>
+        <v>220</v>
+      </c>
+      <c r="C14" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Phil</v>
       </c>
       <c r="D14" t="str" cm="1">
         <f t="array" aca="1" ref="D14" ca="1">IF(_xlfn.XLOOKUP($B14,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B14,wordle_ids,wordles))</f>
-        <v>MOUNT</v>
+        <v>SUGAR</v>
       </c>
       <c r="E14" s="10">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
-        <v>44223</v>
-      </c>
-      <c r="B15" s="4">
-        <v>222</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>6</v>
+      <c r="A15" s="2">
+        <f t="shared" si="0"/>
+        <v>44221</v>
+      </c>
+      <c r="B15" s="6">
+        <f t="shared" si="1"/>
+        <v>220</v>
+      </c>
+      <c r="C15" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Erik</v>
       </c>
       <c r="D15" t="str" cm="1">
         <f t="array" aca="1" ref="D15" ca="1">IF(_xlfn.XLOOKUP($B15,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B15,wordle_ids,wordles))</f>
-        <v>MOUNT</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>18</v>
+        <v>SUGAR</v>
+      </c>
+      <c r="E15" s="10">
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
-        <v>44223</v>
-      </c>
-      <c r="B16" s="4">
-        <v>222</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>7</v>
+      <c r="A16" s="2">
+        <f t="shared" si="0"/>
+        <v>44221</v>
+      </c>
+      <c r="B16" s="6">
+        <f t="shared" si="1"/>
+        <v>220</v>
+      </c>
+      <c r="C16" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>RoBert</v>
       </c>
       <c r="D16" t="str" cm="1">
         <f t="array" aca="1" ref="D16" ca="1">IF(_xlfn.XLOOKUP($B16,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B16,wordle_ids,wordles))</f>
-        <v>MOUNT</v>
+        <v>SUGAR</v>
       </c>
       <c r="E16" s="10">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
-        <v>44223</v>
-      </c>
-      <c r="B17" s="4">
-        <v>222</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>11</v>
+      <c r="A17" s="2">
+        <f t="shared" si="0"/>
+        <v>44221</v>
+      </c>
+      <c r="B17" s="6">
+        <f t="shared" si="1"/>
+        <v>220</v>
+      </c>
+      <c r="C17" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Andrew</v>
       </c>
       <c r="D17" t="str" cm="1">
         <f t="array" aca="1" ref="D17" ca="1">IF(_xlfn.XLOOKUP($B17,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B17,wordle_ids,wordles))</f>
-        <v>MOUNT</v>
-      </c>
-      <c r="E17" s="10">
-        <v>3</v>
-      </c>
+        <v>SUGAR</v>
+      </c>
+      <c r="E17" s="10"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
-        <v>44223</v>
-      </c>
-      <c r="B18" s="4">
-        <v>222</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>12</v>
+      <c r="A18" s="2">
+        <f t="shared" si="0"/>
+        <v>44221</v>
+      </c>
+      <c r="B18" s="6">
+        <f t="shared" si="1"/>
+        <v>220</v>
+      </c>
+      <c r="C18" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Yoyo</v>
       </c>
       <c r="D18" t="str" cm="1">
         <f t="array" aca="1" ref="D18" ca="1">IF(_xlfn.XLOOKUP($B18,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B18,wordle_ids,wordles))</f>
-        <v>MOUNT</v>
-      </c>
-      <c r="E18" s="10">
-        <v>5</v>
-      </c>
+        <v>SUGAR</v>
+      </c>
+      <c r="E18" s="10"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
-        <v>44223</v>
-      </c>
-      <c r="B19" s="4">
-        <v>222</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>13</v>
+      <c r="A19" s="2">
+        <f t="shared" si="0"/>
+        <v>44221</v>
+      </c>
+      <c r="B19" s="6">
+        <f t="shared" si="1"/>
+        <v>220</v>
+      </c>
+      <c r="C19" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Henry</v>
       </c>
       <c r="D19" t="str" cm="1">
         <f t="array" aca="1" ref="D19" ca="1">IF(_xlfn.XLOOKUP($B19,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B19,wordle_ids,wordles))</f>
-        <v>MOUNT</v>
-      </c>
-      <c r="E19" s="10">
-        <v>5</v>
-      </c>
+        <v>SUGAR</v>
+      </c>
+      <c r="E19" s="10"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <f>A14+1</f>
-        <v>44224</v>
+        <f t="shared" si="0"/>
+        <v>44222</v>
       </c>
       <c r="B20" s="6">
-        <f t="shared" ref="B20:B61" si="0">B14+1</f>
-        <v>223</v>
+        <f t="shared" si="1"/>
+        <v>221</v>
       </c>
       <c r="C20" s="2" t="str">
-        <f>C14</f>
+        <f t="shared" si="2"/>
         <v>Phil</v>
       </c>
       <c r="D20" t="str" cm="1">
         <f t="array" aca="1" ref="D20" ca="1">IF(_xlfn.XLOOKUP($B20,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B20,wordle_ids,wordles))</f>
-        <v>PERKY</v>
+        <v>WHACK</v>
       </c>
       <c r="E20" s="10">
         <v>4</v>
@@ -906,20 +933,20 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <f t="shared" ref="A21:A61" si="1">A15+1</f>
-        <v>44224</v>
+        <f t="shared" si="0"/>
+        <v>44222</v>
       </c>
       <c r="B21" s="6">
-        <f t="shared" si="0"/>
-        <v>223</v>
+        <f t="shared" si="1"/>
+        <v>221</v>
       </c>
       <c r="C21" s="2" t="str">
-        <f t="shared" ref="C21:C61" si="2">C15</f>
+        <f t="shared" si="2"/>
         <v>Erik</v>
       </c>
       <c r="D21" t="str" cm="1">
         <f t="array" aca="1" ref="D21" ca="1">IF(_xlfn.XLOOKUP($B21,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B21,wordle_ids,wordles))</f>
-        <v>PERKY</v>
+        <v>WHACK</v>
       </c>
       <c r="E21" s="10">
         <v>5</v>
@@ -927,12 +954,12 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <f t="shared" si="1"/>
-        <v>44224</v>
+        <f t="shared" si="0"/>
+        <v>44222</v>
       </c>
       <c r="B22" s="6">
-        <f t="shared" si="0"/>
-        <v>223</v>
+        <f t="shared" si="1"/>
+        <v>221</v>
       </c>
       <c r="C22" s="2" t="str">
         <f t="shared" si="2"/>
@@ -940,7 +967,7 @@
       </c>
       <c r="D22" t="str" cm="1">
         <f t="array" aca="1" ref="D22" ca="1">IF(_xlfn.XLOOKUP($B22,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B22,wordle_ids,wordles))</f>
-        <v>PERKY</v>
+        <v>WHACK</v>
       </c>
       <c r="E22" s="10">
         <v>4</v>
@@ -948,12 +975,12 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <f t="shared" si="1"/>
-        <v>44224</v>
+        <f t="shared" si="0"/>
+        <v>44222</v>
       </c>
       <c r="B23" s="6">
-        <f t="shared" si="0"/>
-        <v>223</v>
+        <f t="shared" si="1"/>
+        <v>221</v>
       </c>
       <c r="C23" s="2" t="str">
         <f t="shared" si="2"/>
@@ -961,20 +988,18 @@
       </c>
       <c r="D23" t="str" cm="1">
         <f t="array" aca="1" ref="D23" ca="1">IF(_xlfn.XLOOKUP($B23,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B23,wordle_ids,wordles))</f>
-        <v>PERKY</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>18</v>
-      </c>
+        <v>WHACK</v>
+      </c>
+      <c r="E23" s="10"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <f t="shared" si="1"/>
-        <v>44224</v>
+        <f t="shared" si="0"/>
+        <v>44222</v>
       </c>
       <c r="B24" s="6">
-        <f t="shared" si="0"/>
-        <v>223</v>
+        <f t="shared" si="1"/>
+        <v>221</v>
       </c>
       <c r="C24" s="2" t="str">
         <f t="shared" si="2"/>
@@ -982,20 +1007,18 @@
       </c>
       <c r="D24" t="str" cm="1">
         <f t="array" aca="1" ref="D24" ca="1">IF(_xlfn.XLOOKUP($B24,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B24,wordle_ids,wordles))</f>
-        <v>PERKY</v>
-      </c>
-      <c r="E24" s="10">
-        <v>4</v>
-      </c>
+        <v>WHACK</v>
+      </c>
+      <c r="E24" s="10"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <f t="shared" si="1"/>
-        <v>44224</v>
+        <f t="shared" si="0"/>
+        <v>44222</v>
       </c>
       <c r="B25" s="6">
-        <f t="shared" si="0"/>
-        <v>223</v>
+        <f t="shared" si="1"/>
+        <v>221</v>
       </c>
       <c r="C25" s="2" t="str">
         <f t="shared" si="2"/>
@@ -1003,20 +1026,18 @@
       </c>
       <c r="D25" t="str" cm="1">
         <f t="array" aca="1" ref="D25" ca="1">IF(_xlfn.XLOOKUP($B25,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B25,wordle_ids,wordles))</f>
-        <v>PERKY</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>18</v>
-      </c>
+        <v>WHACK</v>
+      </c>
+      <c r="E25" s="10"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <f t="shared" si="1"/>
-        <v>44225</v>
+        <f t="shared" si="0"/>
+        <v>44223</v>
       </c>
       <c r="B26" s="6">
-        <f t="shared" si="0"/>
-        <v>224</v>
+        <f t="shared" si="1"/>
+        <v>222</v>
       </c>
       <c r="C26" s="2" t="str">
         <f t="shared" si="2"/>
@@ -1024,20 +1045,20 @@
       </c>
       <c r="D26" t="str" cm="1">
         <f t="array" aca="1" ref="D26" ca="1">IF(_xlfn.XLOOKUP($B26,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B26,wordle_ids,wordles))</f>
-        <v>COULD</v>
+        <v>MOUNT</v>
       </c>
       <c r="E26" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <f t="shared" si="1"/>
-        <v>44225</v>
+        <f t="shared" si="0"/>
+        <v>44223</v>
       </c>
       <c r="B27" s="6">
-        <f t="shared" si="0"/>
-        <v>224</v>
+        <f t="shared" si="1"/>
+        <v>222</v>
       </c>
       <c r="C27" s="2" t="str">
         <f t="shared" si="2"/>
@@ -1045,20 +1066,20 @@
       </c>
       <c r="D27" t="str" cm="1">
         <f t="array" aca="1" ref="D27" ca="1">IF(_xlfn.XLOOKUP($B27,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B27,wordle_ids,wordles))</f>
-        <v>COULD</v>
-      </c>
-      <c r="E27" s="10">
-        <v>4</v>
+        <v>MOUNT</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <f t="shared" si="1"/>
-        <v>44225</v>
+        <f t="shared" si="0"/>
+        <v>44223</v>
       </c>
       <c r="B28" s="6">
-        <f t="shared" si="0"/>
-        <v>224</v>
+        <f t="shared" si="1"/>
+        <v>222</v>
       </c>
       <c r="C28" s="2" t="str">
         <f t="shared" si="2"/>
@@ -1066,20 +1087,20 @@
       </c>
       <c r="D28" t="str" cm="1">
         <f t="array" aca="1" ref="D28" ca="1">IF(_xlfn.XLOOKUP($B28,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B28,wordle_ids,wordles))</f>
-        <v>COULD</v>
+        <v>MOUNT</v>
       </c>
       <c r="E28" s="10">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <f t="shared" si="1"/>
-        <v>44225</v>
+        <f t="shared" si="0"/>
+        <v>44223</v>
       </c>
       <c r="B29" s="6">
-        <f t="shared" si="0"/>
-        <v>224</v>
+        <f t="shared" si="1"/>
+        <v>222</v>
       </c>
       <c r="C29" s="2" t="str">
         <f t="shared" si="2"/>
@@ -1087,20 +1108,20 @@
       </c>
       <c r="D29" t="str" cm="1">
         <f t="array" aca="1" ref="D29" ca="1">IF(_xlfn.XLOOKUP($B29,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B29,wordle_ids,wordles))</f>
-        <v>COULD</v>
+        <v>MOUNT</v>
       </c>
       <c r="E29" s="10">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <f t="shared" si="1"/>
-        <v>44225</v>
+        <f t="shared" si="0"/>
+        <v>44223</v>
       </c>
       <c r="B30" s="6">
-        <f t="shared" si="0"/>
-        <v>224</v>
+        <f t="shared" si="1"/>
+        <v>222</v>
       </c>
       <c r="C30" s="2" t="str">
         <f t="shared" si="2"/>
@@ -1108,20 +1129,20 @@
       </c>
       <c r="D30" t="str" cm="1">
         <f t="array" aca="1" ref="D30" ca="1">IF(_xlfn.XLOOKUP($B30,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B30,wordle_ids,wordles))</f>
-        <v>COULD</v>
+        <v>MOUNT</v>
       </c>
       <c r="E30" s="10">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <f t="shared" si="1"/>
-        <v>44225</v>
+        <f t="shared" si="0"/>
+        <v>44223</v>
       </c>
       <c r="B31" s="6">
-        <f t="shared" si="0"/>
-        <v>224</v>
+        <f t="shared" si="1"/>
+        <v>222</v>
       </c>
       <c r="C31" s="2" t="str">
         <f t="shared" si="2"/>
@@ -1129,68 +1150,70 @@
       </c>
       <c r="D31" t="str" cm="1">
         <f t="array" aca="1" ref="D31" ca="1">IF(_xlfn.XLOOKUP($B31,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B31,wordle_ids,wordles))</f>
-        <v>COULD</v>
-      </c>
-      <c r="E31" s="10"/>
+        <v>MOUNT</v>
+      </c>
+      <c r="E31" s="10">
+        <v>5</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <f t="shared" si="1"/>
-        <v>44226</v>
+        <f>A26+1</f>
+        <v>44224</v>
       </c>
       <c r="B32" s="6">
-        <f t="shared" si="0"/>
-        <v>225</v>
+        <f t="shared" ref="B32:B91" si="3">B26+1</f>
+        <v>223</v>
       </c>
       <c r="C32" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>C26</f>
         <v>Phil</v>
       </c>
       <c r="D32" t="str" cm="1">
         <f t="array" aca="1" ref="D32" ca="1">IF(_xlfn.XLOOKUP($B32,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B32,wordle_ids,wordles))</f>
-        <v>WRUNG</v>
+        <v>PERKY</v>
       </c>
       <c r="E32" s="10">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <f t="shared" si="1"/>
-        <v>44226</v>
+        <f t="shared" ref="A33:A91" si="4">A27+1</f>
+        <v>44224</v>
       </c>
       <c r="B33" s="6">
-        <f t="shared" si="0"/>
-        <v>225</v>
+        <f t="shared" si="3"/>
+        <v>223</v>
       </c>
       <c r="C33" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="C33:C91" si="5">C27</f>
         <v>Erik</v>
       </c>
       <c r="D33" t="str" cm="1">
         <f t="array" aca="1" ref="D33" ca="1">IF(_xlfn.XLOOKUP($B33,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B33,wordle_ids,wordles))</f>
-        <v>WRUNG</v>
+        <v>PERKY</v>
       </c>
       <c r="E33" s="10">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <f t="shared" si="1"/>
-        <v>44226</v>
+        <f t="shared" si="4"/>
+        <v>44224</v>
       </c>
       <c r="B34" s="6">
-        <f t="shared" si="0"/>
-        <v>225</v>
+        <f t="shared" si="3"/>
+        <v>223</v>
       </c>
       <c r="C34" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>RoBert</v>
       </c>
       <c r="D34" t="str" cm="1">
         <f t="array" aca="1" ref="D34" ca="1">IF(_xlfn.XLOOKUP($B34,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B34,wordle_ids,wordles))</f>
-        <v>WRUNG</v>
+        <v>PERKY</v>
       </c>
       <c r="E34" s="10">
         <v>4</v>
@@ -1198,41 +1221,41 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
-        <f t="shared" si="1"/>
-        <v>44226</v>
+        <f t="shared" si="4"/>
+        <v>44224</v>
       </c>
       <c r="B35" s="6">
-        <f t="shared" si="0"/>
-        <v>225</v>
+        <f t="shared" si="3"/>
+        <v>223</v>
       </c>
       <c r="C35" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Andrew</v>
       </c>
       <c r="D35" t="str" cm="1">
         <f t="array" aca="1" ref="D35" ca="1">IF(_xlfn.XLOOKUP($B35,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B35,wordle_ids,wordles))</f>
-        <v>WRUNG</v>
-      </c>
-      <c r="E35" s="10">
-        <v>4</v>
+        <v>PERKY</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
-        <f t="shared" si="1"/>
-        <v>44226</v>
+        <f t="shared" si="4"/>
+        <v>44224</v>
       </c>
       <c r="B36" s="6">
-        <f t="shared" si="0"/>
-        <v>225</v>
+        <f t="shared" si="3"/>
+        <v>223</v>
       </c>
       <c r="C36" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Yoyo</v>
       </c>
       <c r="D36" t="str" cm="1">
         <f t="array" aca="1" ref="D36" ca="1">IF(_xlfn.XLOOKUP($B36,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B36,wordle_ids,wordles))</f>
-        <v>WRUNG</v>
+        <v>PERKY</v>
       </c>
       <c r="E36" s="10">
         <v>4</v>
@@ -1240,60 +1263,62 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
-        <f t="shared" si="1"/>
-        <v>44226</v>
+        <f t="shared" si="4"/>
+        <v>44224</v>
       </c>
       <c r="B37" s="6">
-        <f t="shared" si="0"/>
-        <v>225</v>
+        <f t="shared" si="3"/>
+        <v>223</v>
       </c>
       <c r="C37" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Henry</v>
       </c>
       <c r="D37" t="str" cm="1">
         <f t="array" aca="1" ref="D37" ca="1">IF(_xlfn.XLOOKUP($B37,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B37,wordle_ids,wordles))</f>
-        <v>WRUNG</v>
-      </c>
-      <c r="E37" s="10"/>
+        <v>PERKY</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
-        <f t="shared" si="1"/>
-        <v>44227</v>
+        <f t="shared" si="4"/>
+        <v>44225</v>
       </c>
       <c r="B38" s="6">
-        <f t="shared" si="0"/>
-        <v>226</v>
+        <f t="shared" si="3"/>
+        <v>224</v>
       </c>
       <c r="C38" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Phil</v>
       </c>
       <c r="D38" t="str" cm="1">
         <f t="array" aca="1" ref="D38" ca="1">IF(_xlfn.XLOOKUP($B38,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B38,wordle_ids,wordles))</f>
-        <v>LIGHT</v>
+        <v>COULD</v>
       </c>
       <c r="E38" s="10">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
-        <f t="shared" si="1"/>
-        <v>44227</v>
+        <f t="shared" si="4"/>
+        <v>44225</v>
       </c>
       <c r="B39" s="6">
-        <f t="shared" si="0"/>
-        <v>226</v>
+        <f t="shared" si="3"/>
+        <v>224</v>
       </c>
       <c r="C39" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Erik</v>
       </c>
       <c r="D39" t="str" cm="1">
         <f t="array" aca="1" ref="D39" ca="1">IF(_xlfn.XLOOKUP($B39,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B39,wordle_ids,wordles))</f>
-        <v>LIGHT</v>
+        <v>COULD</v>
       </c>
       <c r="E39" s="10">
         <v>4</v>
@@ -1301,41 +1326,41 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
-        <f t="shared" si="1"/>
-        <v>44227</v>
+        <f t="shared" si="4"/>
+        <v>44225</v>
       </c>
       <c r="B40" s="6">
-        <f t="shared" si="0"/>
-        <v>226</v>
+        <f t="shared" si="3"/>
+        <v>224</v>
       </c>
       <c r="C40" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>RoBert</v>
       </c>
       <c r="D40" t="str" cm="1">
         <f t="array" aca="1" ref="D40" ca="1">IF(_xlfn.XLOOKUP($B40,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B40,wordle_ids,wordles))</f>
-        <v>LIGHT</v>
+        <v>COULD</v>
       </c>
       <c r="E40" s="10">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
-        <f t="shared" si="1"/>
-        <v>44227</v>
+        <f t="shared" si="4"/>
+        <v>44225</v>
       </c>
       <c r="B41" s="6">
-        <f t="shared" si="0"/>
-        <v>226</v>
+        <f t="shared" si="3"/>
+        <v>224</v>
       </c>
       <c r="C41" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Andrew</v>
       </c>
       <c r="D41" t="str" cm="1">
         <f t="array" aca="1" ref="D41" ca="1">IF(_xlfn.XLOOKUP($B41,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B41,wordle_ids,wordles))</f>
-        <v>LIGHT</v>
+        <v>COULD</v>
       </c>
       <c r="E41" s="10">
         <v>5</v>
@@ -1343,20 +1368,20 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
-        <f t="shared" si="1"/>
-        <v>44227</v>
+        <f t="shared" si="4"/>
+        <v>44225</v>
       </c>
       <c r="B42" s="6">
-        <f t="shared" si="0"/>
-        <v>226</v>
+        <f t="shared" si="3"/>
+        <v>224</v>
       </c>
       <c r="C42" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Yoyo</v>
       </c>
       <c r="D42" t="str" cm="1">
         <f t="array" aca="1" ref="D42" ca="1">IF(_xlfn.XLOOKUP($B42,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B42,wordle_ids,wordles))</f>
-        <v>LIGHT</v>
+        <v>COULD</v>
       </c>
       <c r="E42" s="10">
         <v>4</v>
@@ -1364,104 +1389,102 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
-        <f>A37+1</f>
-        <v>44227</v>
+        <f t="shared" si="4"/>
+        <v>44225</v>
       </c>
       <c r="B43" s="6">
-        <f t="shared" si="0"/>
-        <v>226</v>
+        <f t="shared" si="3"/>
+        <v>224</v>
       </c>
       <c r="C43" s="2" t="str">
-        <f>C37</f>
+        <f t="shared" si="5"/>
         <v>Henry</v>
       </c>
       <c r="D43" t="str" cm="1">
         <f t="array" aca="1" ref="D43" ca="1">IF(_xlfn.XLOOKUP($B43,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B43,wordle_ids,wordles))</f>
-        <v>LIGHT</v>
-      </c>
-      <c r="E43" s="10">
-        <v>6</v>
-      </c>
+        <v>COULD</v>
+      </c>
+      <c r="E43" s="10"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
-        <f t="shared" si="1"/>
-        <v>44228</v>
+        <f t="shared" si="4"/>
+        <v>44226</v>
       </c>
       <c r="B44" s="6">
-        <f t="shared" si="0"/>
-        <v>227</v>
+        <f t="shared" si="3"/>
+        <v>225</v>
       </c>
       <c r="C44" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Phil</v>
       </c>
       <c r="D44" t="str" cm="1">
         <f t="array" aca="1" ref="D44" ca="1">IF(_xlfn.XLOOKUP($B44,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B44,wordle_ids,wordles))</f>
-        <v>THOSE</v>
+        <v>WRUNG</v>
       </c>
       <c r="E44" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
-        <f t="shared" si="1"/>
-        <v>44228</v>
+        <f t="shared" si="4"/>
+        <v>44226</v>
       </c>
       <c r="B45" s="6">
-        <f t="shared" si="0"/>
-        <v>227</v>
+        <f t="shared" si="3"/>
+        <v>225</v>
       </c>
       <c r="C45" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Erik</v>
       </c>
       <c r="D45" t="str" cm="1">
         <f t="array" aca="1" ref="D45" ca="1">IF(_xlfn.XLOOKUP($B45,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B45,wordle_ids,wordles))</f>
-        <v>THOSE</v>
+        <v>WRUNG</v>
       </c>
       <c r="E45" s="10">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
-        <f t="shared" si="1"/>
-        <v>44228</v>
+        <f t="shared" si="4"/>
+        <v>44226</v>
       </c>
       <c r="B46" s="6">
-        <f t="shared" si="0"/>
-        <v>227</v>
+        <f t="shared" si="3"/>
+        <v>225</v>
       </c>
       <c r="C46" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>RoBert</v>
       </c>
       <c r="D46" t="str" cm="1">
         <f t="array" aca="1" ref="D46" ca="1">IF(_xlfn.XLOOKUP($B46,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B46,wordle_ids,wordles))</f>
-        <v>THOSE</v>
+        <v>WRUNG</v>
       </c>
       <c r="E46" s="10">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
-        <f t="shared" si="1"/>
-        <v>44228</v>
+        <f t="shared" si="4"/>
+        <v>44226</v>
       </c>
       <c r="B47" s="6">
-        <f t="shared" si="0"/>
-        <v>227</v>
+        <f t="shared" si="3"/>
+        <v>225</v>
       </c>
       <c r="C47" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Andrew</v>
       </c>
       <c r="D47" t="str" cm="1">
         <f t="array" aca="1" ref="D47" ca="1">IF(_xlfn.XLOOKUP($B47,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B47,wordle_ids,wordles))</f>
-        <v>THOSE</v>
+        <v>WRUNG</v>
       </c>
       <c r="E47" s="10">
         <v>4</v>
@@ -1469,104 +1492,102 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
-        <f t="shared" si="1"/>
-        <v>44228</v>
+        <f t="shared" si="4"/>
+        <v>44226</v>
       </c>
       <c r="B48" s="6">
-        <f t="shared" si="0"/>
-        <v>227</v>
+        <f t="shared" si="3"/>
+        <v>225</v>
       </c>
       <c r="C48" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Yoyo</v>
       </c>
       <c r="D48" t="str" cm="1">
         <f t="array" aca="1" ref="D48" ca="1">IF(_xlfn.XLOOKUP($B48,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B48,wordle_ids,wordles))</f>
-        <v>THOSE</v>
+        <v>WRUNG</v>
       </c>
       <c r="E48" s="10">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
-        <f t="shared" si="1"/>
-        <v>44228</v>
+        <f t="shared" si="4"/>
+        <v>44226</v>
       </c>
       <c r="B49" s="6">
-        <f t="shared" si="0"/>
-        <v>227</v>
+        <f t="shared" si="3"/>
+        <v>225</v>
       </c>
       <c r="C49" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Henry</v>
       </c>
       <c r="D49" t="str" cm="1">
         <f t="array" aca="1" ref="D49" ca="1">IF(_xlfn.XLOOKUP($B49,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B49,wordle_ids,wordles))</f>
-        <v>THOSE</v>
-      </c>
-      <c r="E49" s="10">
-        <v>3</v>
-      </c>
+        <v>WRUNG</v>
+      </c>
+      <c r="E49" s="10"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
-        <f t="shared" si="1"/>
-        <v>44229</v>
+        <f t="shared" si="4"/>
+        <v>44227</v>
       </c>
       <c r="B50" s="6">
-        <f t="shared" si="0"/>
-        <v>228</v>
+        <f t="shared" si="3"/>
+        <v>226</v>
       </c>
       <c r="C50" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Phil</v>
       </c>
       <c r="D50" t="str" cm="1">
         <f t="array" aca="1" ref="D50" ca="1">IF(_xlfn.XLOOKUP($B50,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B50,wordle_ids,wordles))</f>
-        <v>MOIST</v>
+        <v>LIGHT</v>
       </c>
       <c r="E50" s="10">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
-        <f t="shared" si="1"/>
-        <v>44229</v>
+        <f t="shared" si="4"/>
+        <v>44227</v>
       </c>
       <c r="B51" s="6">
-        <f t="shared" si="0"/>
-        <v>228</v>
+        <f t="shared" si="3"/>
+        <v>226</v>
       </c>
       <c r="C51" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Erik</v>
       </c>
       <c r="D51" t="str" cm="1">
         <f t="array" aca="1" ref="D51" ca="1">IF(_xlfn.XLOOKUP($B51,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B51,wordle_ids,wordles))</f>
-        <v>MOIST</v>
+        <v>LIGHT</v>
       </c>
       <c r="E51" s="10">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
-        <f t="shared" si="1"/>
-        <v>44229</v>
+        <f t="shared" si="4"/>
+        <v>44227</v>
       </c>
       <c r="B52" s="6">
-        <f t="shared" si="0"/>
-        <v>228</v>
+        <f t="shared" si="3"/>
+        <v>226</v>
       </c>
       <c r="C52" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>RoBert</v>
       </c>
       <c r="D52" t="str" cm="1">
         <f t="array" aca="1" ref="D52" ca="1">IF(_xlfn.XLOOKUP($B52,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B52,wordle_ids,wordles))</f>
-        <v>MOIST</v>
+        <v>LIGHT</v>
       </c>
       <c r="E52" s="10">
         <v>3</v>
@@ -1574,41 +1595,41 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
-        <f t="shared" si="1"/>
-        <v>44229</v>
+        <f t="shared" si="4"/>
+        <v>44227</v>
       </c>
       <c r="B53" s="6">
-        <f t="shared" si="0"/>
-        <v>228</v>
+        <f t="shared" si="3"/>
+        <v>226</v>
       </c>
       <c r="C53" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Andrew</v>
       </c>
       <c r="D53" t="str" cm="1">
         <f t="array" aca="1" ref="D53" ca="1">IF(_xlfn.XLOOKUP($B53,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B53,wordle_ids,wordles))</f>
-        <v>MOIST</v>
+        <v>LIGHT</v>
       </c>
       <c r="E53" s="10">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
-        <f t="shared" si="1"/>
-        <v>44229</v>
+        <f t="shared" si="4"/>
+        <v>44227</v>
       </c>
       <c r="B54" s="6">
-        <f t="shared" si="0"/>
-        <v>228</v>
+        <f t="shared" si="3"/>
+        <v>226</v>
       </c>
       <c r="C54" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Yoyo</v>
       </c>
       <c r="D54" t="str" cm="1">
         <f t="array" aca="1" ref="D54" ca="1">IF(_xlfn.XLOOKUP($B54,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B54,wordle_ids,wordles))</f>
-        <v>MOIST</v>
+        <v>LIGHT</v>
       </c>
       <c r="E54" s="10">
         <v>4</v>
@@ -1616,20 +1637,20 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
-        <f t="shared" si="1"/>
-        <v>44229</v>
+        <f>A49+1</f>
+        <v>44227</v>
       </c>
       <c r="B55" s="6">
-        <f t="shared" si="0"/>
-        <v>228</v>
+        <f t="shared" si="3"/>
+        <v>226</v>
       </c>
       <c r="C55" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>C49</f>
         <v>Henry</v>
       </c>
       <c r="D55" t="str" cm="1">
         <f t="array" aca="1" ref="D55" ca="1">IF(_xlfn.XLOOKUP($B55,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B55,wordle_ids,wordles))</f>
-        <v>MOIST</v>
+        <v>LIGHT</v>
       </c>
       <c r="E55" s="10">
         <v>6</v>
@@ -1637,83 +1658,83 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
-        <f t="shared" si="1"/>
-        <v>44230</v>
+        <f t="shared" si="4"/>
+        <v>44228</v>
       </c>
       <c r="B56" s="6">
-        <f t="shared" si="0"/>
-        <v>229</v>
+        <f t="shared" si="3"/>
+        <v>227</v>
       </c>
       <c r="C56" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Phil</v>
       </c>
       <c r="D56" t="str" cm="1">
         <f t="array" aca="1" ref="D56" ca="1">IF(_xlfn.XLOOKUP($B56,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B56,wordle_ids,wordles))</f>
-        <v>SHARD</v>
+        <v>THOSE</v>
       </c>
       <c r="E56" s="10">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
-        <f t="shared" si="1"/>
-        <v>44230</v>
+        <f t="shared" si="4"/>
+        <v>44228</v>
       </c>
       <c r="B57" s="6">
-        <f t="shared" si="0"/>
-        <v>229</v>
+        <f t="shared" si="3"/>
+        <v>227</v>
       </c>
       <c r="C57" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Erik</v>
       </c>
       <c r="D57" t="str" cm="1">
         <f t="array" aca="1" ref="D57" ca="1">IF(_xlfn.XLOOKUP($B57,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B57,wordle_ids,wordles))</f>
-        <v>SHARD</v>
+        <v>THOSE</v>
       </c>
       <c r="E57" s="10">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
-        <f t="shared" si="1"/>
-        <v>44230</v>
+        <f t="shared" si="4"/>
+        <v>44228</v>
       </c>
       <c r="B58" s="6">
-        <f t="shared" si="0"/>
-        <v>229</v>
+        <f t="shared" si="3"/>
+        <v>227</v>
       </c>
       <c r="C58" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>RoBert</v>
       </c>
       <c r="D58" t="str" cm="1">
         <f t="array" aca="1" ref="D58" ca="1">IF(_xlfn.XLOOKUP($B58,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B58,wordle_ids,wordles))</f>
-        <v>SHARD</v>
+        <v>THOSE</v>
       </c>
       <c r="E58" s="10">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
-        <f t="shared" si="1"/>
-        <v>44230</v>
+        <f t="shared" si="4"/>
+        <v>44228</v>
       </c>
       <c r="B59" s="6">
-        <f t="shared" si="0"/>
-        <v>229</v>
+        <f t="shared" si="3"/>
+        <v>227</v>
       </c>
       <c r="C59" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Andrew</v>
       </c>
       <c r="D59" t="str" cm="1">
         <f t="array" aca="1" ref="D59" ca="1">IF(_xlfn.XLOOKUP($B59,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B59,wordle_ids,wordles))</f>
-        <v>SHARD</v>
+        <v>THOSE</v>
       </c>
       <c r="E59" s="10">
         <v>4</v>
@@ -1721,149 +1742,698 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
-        <f t="shared" si="1"/>
-        <v>44230</v>
+        <f t="shared" si="4"/>
+        <v>44228</v>
       </c>
       <c r="B60" s="6">
-        <f t="shared" si="0"/>
-        <v>229</v>
+        <f t="shared" si="3"/>
+        <v>227</v>
       </c>
       <c r="C60" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Yoyo</v>
       </c>
       <c r="D60" t="str" cm="1">
         <f t="array" aca="1" ref="D60" ca="1">IF(_xlfn.XLOOKUP($B60,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B60,wordle_ids,wordles))</f>
-        <v>SHARD</v>
+        <v>THOSE</v>
       </c>
       <c r="E60" s="10">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
-        <f t="shared" si="1"/>
-        <v>44230</v>
+        <f t="shared" si="4"/>
+        <v>44228</v>
       </c>
       <c r="B61" s="6">
-        <f t="shared" si="0"/>
-        <v>229</v>
+        <f t="shared" si="3"/>
+        <v>227</v>
       </c>
       <c r="C61" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>Henry</v>
       </c>
       <c r="D61" t="str" cm="1">
         <f t="array" aca="1" ref="D61" ca="1">IF(_xlfn.XLOOKUP($B61,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B61,wordle_ids,wordles))</f>
+        <v>THOSE</v>
+      </c>
+      <c r="E61" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
+        <f t="shared" si="4"/>
+        <v>44229</v>
+      </c>
+      <c r="B62" s="6">
+        <f t="shared" si="3"/>
+        <v>228</v>
+      </c>
+      <c r="C62" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>Phil</v>
+      </c>
+      <c r="D62" t="str" cm="1">
+        <f t="array" aca="1" ref="D62" ca="1">IF(_xlfn.XLOOKUP($B62,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B62,wordle_ids,wordles))</f>
+        <v>MOIST</v>
+      </c>
+      <c r="E62" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="2">
+        <f t="shared" si="4"/>
+        <v>44229</v>
+      </c>
+      <c r="B63" s="6">
+        <f t="shared" si="3"/>
+        <v>228</v>
+      </c>
+      <c r="C63" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>Erik</v>
+      </c>
+      <c r="D63" t="str" cm="1">
+        <f t="array" aca="1" ref="D63" ca="1">IF(_xlfn.XLOOKUP($B63,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B63,wordle_ids,wordles))</f>
+        <v>MOIST</v>
+      </c>
+      <c r="E63" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="2">
+        <f t="shared" si="4"/>
+        <v>44229</v>
+      </c>
+      <c r="B64" s="6">
+        <f t="shared" si="3"/>
+        <v>228</v>
+      </c>
+      <c r="C64" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>RoBert</v>
+      </c>
+      <c r="D64" t="str" cm="1">
+        <f t="array" aca="1" ref="D64" ca="1">IF(_xlfn.XLOOKUP($B64,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B64,wordle_ids,wordles))</f>
+        <v>MOIST</v>
+      </c>
+      <c r="E64" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="2">
+        <f t="shared" si="4"/>
+        <v>44229</v>
+      </c>
+      <c r="B65" s="6">
+        <f t="shared" si="3"/>
+        <v>228</v>
+      </c>
+      <c r="C65" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>Andrew</v>
+      </c>
+      <c r="D65" t="str" cm="1">
+        <f t="array" aca="1" ref="D65" ca="1">IF(_xlfn.XLOOKUP($B65,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B65,wordle_ids,wordles))</f>
+        <v>MOIST</v>
+      </c>
+      <c r="E65" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="2">
+        <f t="shared" si="4"/>
+        <v>44229</v>
+      </c>
+      <c r="B66" s="6">
+        <f t="shared" si="3"/>
+        <v>228</v>
+      </c>
+      <c r="C66" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>Yoyo</v>
+      </c>
+      <c r="D66" t="str" cm="1">
+        <f t="array" aca="1" ref="D66" ca="1">IF(_xlfn.XLOOKUP($B66,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B66,wordle_ids,wordles))</f>
+        <v>MOIST</v>
+      </c>
+      <c r="E66" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="2">
+        <f t="shared" si="4"/>
+        <v>44229</v>
+      </c>
+      <c r="B67" s="6">
+        <f t="shared" si="3"/>
+        <v>228</v>
+      </c>
+      <c r="C67" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>Henry</v>
+      </c>
+      <c r="D67" t="str" cm="1">
+        <f t="array" aca="1" ref="D67" ca="1">IF(_xlfn.XLOOKUP($B67,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B67,wordle_ids,wordles))</f>
+        <v>MOIST</v>
+      </c>
+      <c r="E67" s="10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="2">
+        <f t="shared" si="4"/>
+        <v>44230</v>
+      </c>
+      <c r="B68" s="6">
+        <f t="shared" si="3"/>
+        <v>229</v>
+      </c>
+      <c r="C68" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>Phil</v>
+      </c>
+      <c r="D68" t="str" cm="1">
+        <f t="array" aca="1" ref="D68" ca="1">IF(_xlfn.XLOOKUP($B68,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B68,wordle_ids,wordles))</f>
         <v>SHARD</v>
       </c>
-      <c r="E61" s="10">
+      <c r="E68" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="2">
+        <f t="shared" si="4"/>
+        <v>44230</v>
+      </c>
+      <c r="B69" s="6">
+        <f t="shared" si="3"/>
+        <v>229</v>
+      </c>
+      <c r="C69" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>Erik</v>
+      </c>
+      <c r="D69" t="str" cm="1">
+        <f t="array" aca="1" ref="D69" ca="1">IF(_xlfn.XLOOKUP($B69,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B69,wordle_ids,wordles))</f>
+        <v>SHARD</v>
+      </c>
+      <c r="E69" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="2">
+        <f t="shared" si="4"/>
+        <v>44230</v>
+      </c>
+      <c r="B70" s="6">
+        <f t="shared" si="3"/>
+        <v>229</v>
+      </c>
+      <c r="C70" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>RoBert</v>
+      </c>
+      <c r="D70" t="str" cm="1">
+        <f t="array" aca="1" ref="D70" ca="1">IF(_xlfn.XLOOKUP($B70,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B70,wordle_ids,wordles))</f>
+        <v>SHARD</v>
+      </c>
+      <c r="E70" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="2">
+        <f t="shared" si="4"/>
+        <v>44230</v>
+      </c>
+      <c r="B71" s="6">
+        <f t="shared" si="3"/>
+        <v>229</v>
+      </c>
+      <c r="C71" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>Andrew</v>
+      </c>
+      <c r="D71" t="str" cm="1">
+        <f t="array" aca="1" ref="D71" ca="1">IF(_xlfn.XLOOKUP($B71,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B71,wordle_ids,wordles))</f>
+        <v>SHARD</v>
+      </c>
+      <c r="E71" s="10">
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E62" s="10"/>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E63" s="10"/>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E64" s="10"/>
-    </row>
-    <row r="65" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E65" s="10"/>
-    </row>
-    <row r="66" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E66" s="10"/>
-    </row>
-    <row r="67" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E67" s="10"/>
-    </row>
-    <row r="68" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E68" s="10"/>
-    </row>
-    <row r="69" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E69" s="10"/>
-    </row>
-    <row r="70" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E70" s="10"/>
-    </row>
-    <row r="71" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E71" s="10"/>
-    </row>
-    <row r="72" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E72" s="10"/>
-    </row>
-    <row r="73" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E73" s="10"/>
-    </row>
-    <row r="74" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E74" s="10"/>
-    </row>
-    <row r="75" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E75" s="10"/>
-    </row>
-    <row r="76" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E76" s="10"/>
-    </row>
-    <row r="77" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E77" s="10"/>
-    </row>
-    <row r="78" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E78" s="10"/>
-    </row>
-    <row r="79" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E79" s="10"/>
-    </row>
-    <row r="80" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E80" s="10"/>
-    </row>
-    <row r="81" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E81" s="10"/>
-    </row>
-    <row r="82" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E82" s="10"/>
-    </row>
-    <row r="83" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E83" s="10"/>
-    </row>
-    <row r="84" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E84" s="10"/>
-    </row>
-    <row r="85" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E85" s="10"/>
-    </row>
-    <row r="86" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E86" s="10"/>
-    </row>
-    <row r="87" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E87" s="10"/>
-    </row>
-    <row r="88" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E88" s="10"/>
-    </row>
-    <row r="89" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E89" s="10"/>
-    </row>
-    <row r="90" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E90" s="10"/>
-    </row>
-    <row r="91" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E91" s="10"/>
-    </row>
-    <row r="92" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="2">
+        <f t="shared" si="4"/>
+        <v>44230</v>
+      </c>
+      <c r="B72" s="6">
+        <f t="shared" si="3"/>
+        <v>229</v>
+      </c>
+      <c r="C72" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>Yoyo</v>
+      </c>
+      <c r="D72" t="str" cm="1">
+        <f t="array" aca="1" ref="D72" ca="1">IF(_xlfn.XLOOKUP($B72,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B72,wordle_ids,wordles))</f>
+        <v>SHARD</v>
+      </c>
+      <c r="E72" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="2">
+        <f t="shared" si="4"/>
+        <v>44230</v>
+      </c>
+      <c r="B73" s="6">
+        <f t="shared" si="3"/>
+        <v>229</v>
+      </c>
+      <c r="C73" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>Henry</v>
+      </c>
+      <c r="D73" t="str" cm="1">
+        <f t="array" aca="1" ref="D73" ca="1">IF(_xlfn.XLOOKUP($B73,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B73,wordle_ids,wordles))</f>
+        <v>SHARD</v>
+      </c>
+      <c r="E73" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="2">
+        <f t="shared" si="4"/>
+        <v>44231</v>
+      </c>
+      <c r="B74" s="6">
+        <f t="shared" si="3"/>
+        <v>230</v>
+      </c>
+      <c r="C74" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>Phil</v>
+      </c>
+      <c r="D74" t="str" cm="1">
+        <f t="array" aca="1" ref="D74" ca="1">IF(_xlfn.XLOOKUP($B74,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B74,wordle_ids,wordles))</f>
+        <v>PLEAT</v>
+      </c>
+      <c r="E74" s="10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="2">
+        <f t="shared" si="4"/>
+        <v>44231</v>
+      </c>
+      <c r="B75" s="6">
+        <f t="shared" si="3"/>
+        <v>230</v>
+      </c>
+      <c r="C75" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>Erik</v>
+      </c>
+      <c r="D75" t="str" cm="1">
+        <f t="array" aca="1" ref="D75" ca="1">IF(_xlfn.XLOOKUP($B75,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B75,wordle_ids,wordles))</f>
+        <v>PLEAT</v>
+      </c>
+      <c r="E75" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="2">
+        <f t="shared" si="4"/>
+        <v>44231</v>
+      </c>
+      <c r="B76" s="6">
+        <f t="shared" si="3"/>
+        <v>230</v>
+      </c>
+      <c r="C76" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>RoBert</v>
+      </c>
+      <c r="D76" t="str" cm="1">
+        <f t="array" aca="1" ref="D76" ca="1">IF(_xlfn.XLOOKUP($B76,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B76,wordle_ids,wordles))</f>
+        <v>PLEAT</v>
+      </c>
+      <c r="E76" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="2">
+        <f t="shared" si="4"/>
+        <v>44231</v>
+      </c>
+      <c r="B77" s="6">
+        <f t="shared" si="3"/>
+        <v>230</v>
+      </c>
+      <c r="C77" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>Andrew</v>
+      </c>
+      <c r="D77" t="str" cm="1">
+        <f t="array" aca="1" ref="D77" ca="1">IF(_xlfn.XLOOKUP($B77,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B77,wordle_ids,wordles))</f>
+        <v>PLEAT</v>
+      </c>
+      <c r="E77" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="2">
+        <f t="shared" si="4"/>
+        <v>44231</v>
+      </c>
+      <c r="B78" s="6">
+        <f t="shared" si="3"/>
+        <v>230</v>
+      </c>
+      <c r="C78" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>Yoyo</v>
+      </c>
+      <c r="D78" t="str" cm="1">
+        <f t="array" aca="1" ref="D78" ca="1">IF(_xlfn.XLOOKUP($B78,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B78,wordle_ids,wordles))</f>
+        <v>PLEAT</v>
+      </c>
+      <c r="E78" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="2">
+        <f t="shared" si="4"/>
+        <v>44231</v>
+      </c>
+      <c r="B79" s="6">
+        <f t="shared" si="3"/>
+        <v>230</v>
+      </c>
+      <c r="C79" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>Henry</v>
+      </c>
+      <c r="D79" t="str" cm="1">
+        <f t="array" aca="1" ref="D79" ca="1">IF(_xlfn.XLOOKUP($B79,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B79,wordle_ids,wordles))</f>
+        <v>PLEAT</v>
+      </c>
+      <c r="E79" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="2">
+        <f t="shared" si="4"/>
+        <v>44232</v>
+      </c>
+      <c r="B80" s="6">
+        <f t="shared" si="3"/>
+        <v>231</v>
+      </c>
+      <c r="C80" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>Phil</v>
+      </c>
+      <c r="D80" t="str" cm="1">
+        <f t="array" aca="1" ref="D80" ca="1">IF(_xlfn.XLOOKUP($B80,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B80,wordle_ids,wordles))</f>
+        <v>ALOFT</v>
+      </c>
+      <c r="E80" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="2">
+        <f t="shared" si="4"/>
+        <v>44232</v>
+      </c>
+      <c r="B81" s="6">
+        <f t="shared" si="3"/>
+        <v>231</v>
+      </c>
+      <c r="C81" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>Erik</v>
+      </c>
+      <c r="D81" t="str" cm="1">
+        <f t="array" aca="1" ref="D81" ca="1">IF(_xlfn.XLOOKUP($B81,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B81,wordle_ids,wordles))</f>
+        <v>ALOFT</v>
+      </c>
+      <c r="E81" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="2">
+        <f t="shared" si="4"/>
+        <v>44232</v>
+      </c>
+      <c r="B82" s="6">
+        <f t="shared" si="3"/>
+        <v>231</v>
+      </c>
+      <c r="C82" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>RoBert</v>
+      </c>
+      <c r="D82" t="str" cm="1">
+        <f t="array" aca="1" ref="D82" ca="1">IF(_xlfn.XLOOKUP($B82,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B82,wordle_ids,wordles))</f>
+        <v>ALOFT</v>
+      </c>
+      <c r="E82" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="2">
+        <f t="shared" si="4"/>
+        <v>44232</v>
+      </c>
+      <c r="B83" s="6">
+        <f t="shared" si="3"/>
+        <v>231</v>
+      </c>
+      <c r="C83" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>Andrew</v>
+      </c>
+      <c r="D83" t="str" cm="1">
+        <f t="array" aca="1" ref="D83" ca="1">IF(_xlfn.XLOOKUP($B83,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B83,wordle_ids,wordles))</f>
+        <v>ALOFT</v>
+      </c>
+      <c r="E83" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="2">
+        <f t="shared" si="4"/>
+        <v>44232</v>
+      </c>
+      <c r="B84" s="6">
+        <f t="shared" si="3"/>
+        <v>231</v>
+      </c>
+      <c r="C84" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>Yoyo</v>
+      </c>
+      <c r="D84" t="str" cm="1">
+        <f t="array" aca="1" ref="D84" ca="1">IF(_xlfn.XLOOKUP($B84,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B84,wordle_ids,wordles))</f>
+        <v>ALOFT</v>
+      </c>
+      <c r="E84" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="2">
+        <f t="shared" si="4"/>
+        <v>44232</v>
+      </c>
+      <c r="B85" s="6">
+        <f t="shared" si="3"/>
+        <v>231</v>
+      </c>
+      <c r="C85" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>Henry</v>
+      </c>
+      <c r="D85" t="str" cm="1">
+        <f t="array" aca="1" ref="D85" ca="1">IF(_xlfn.XLOOKUP($B85,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B85,wordle_ids,wordles))</f>
+        <v>ALOFT</v>
+      </c>
+      <c r="E85" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="2">
+        <f t="shared" si="4"/>
+        <v>44233</v>
+      </c>
+      <c r="B86" s="6">
+        <f t="shared" si="3"/>
+        <v>232</v>
+      </c>
+      <c r="C86" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>Phil</v>
+      </c>
+      <c r="D86" t="str" cm="1">
+        <f t="array" aca="1" ref="D86" ca="1">IF(_xlfn.XLOOKUP($B86,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B86,wordle_ids,wordles))</f>
+        <v>SKILL</v>
+      </c>
+      <c r="E86" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="2">
+        <f t="shared" si="4"/>
+        <v>44233</v>
+      </c>
+      <c r="B87" s="6">
+        <f t="shared" si="3"/>
+        <v>232</v>
+      </c>
+      <c r="C87" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>Erik</v>
+      </c>
+      <c r="D87" t="str" cm="1">
+        <f t="array" aca="1" ref="D87" ca="1">IF(_xlfn.XLOOKUP($B87,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B87,wordle_ids,wordles))</f>
+        <v>SKILL</v>
+      </c>
+      <c r="E87" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="2">
+        <f t="shared" si="4"/>
+        <v>44233</v>
+      </c>
+      <c r="B88" s="6">
+        <f t="shared" si="3"/>
+        <v>232</v>
+      </c>
+      <c r="C88" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>RoBert</v>
+      </c>
+      <c r="D88" t="str" cm="1">
+        <f t="array" aca="1" ref="D88" ca="1">IF(_xlfn.XLOOKUP($B88,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B88,wordle_ids,wordles))</f>
+        <v>SKILL</v>
+      </c>
+      <c r="E88" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="2">
+        <f t="shared" si="4"/>
+        <v>44233</v>
+      </c>
+      <c r="B89" s="6">
+        <f t="shared" si="3"/>
+        <v>232</v>
+      </c>
+      <c r="C89" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>Andrew</v>
+      </c>
+      <c r="D89" t="str" cm="1">
+        <f t="array" aca="1" ref="D89" ca="1">IF(_xlfn.XLOOKUP($B89,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B89,wordle_ids,wordles))</f>
+        <v>SKILL</v>
+      </c>
+      <c r="E89" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="2">
+        <f t="shared" si="4"/>
+        <v>44233</v>
+      </c>
+      <c r="B90" s="6">
+        <f t="shared" si="3"/>
+        <v>232</v>
+      </c>
+      <c r="C90" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>Yoyo</v>
+      </c>
+      <c r="D90" t="str" cm="1">
+        <f t="array" aca="1" ref="D90" ca="1">IF(_xlfn.XLOOKUP($B90,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B90,wordle_ids,wordles))</f>
+        <v>SKILL</v>
+      </c>
+      <c r="E90" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="2">
+        <f t="shared" si="4"/>
+        <v>44233</v>
+      </c>
+      <c r="B91" s="6">
+        <f t="shared" si="3"/>
+        <v>232</v>
+      </c>
+      <c r="C91" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>Henry</v>
+      </c>
+      <c r="D91" t="str" cm="1">
+        <f t="array" aca="1" ref="D91" ca="1">IF(_xlfn.XLOOKUP($B91,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B91,wordle_ids,wordles))</f>
+        <v>SKILL</v>
+      </c>
+      <c r="E91" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="2"/>
+      <c r="B92" s="6"/>
+      <c r="C92" s="2"/>
       <c r="E92" s="10"/>
     </row>
-    <row r="93" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="2"/>
+      <c r="B93" s="6"/>
+      <c r="C93" s="2"/>
       <c r="E93" s="10"/>
     </row>
-    <row r="94" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="2"/>
+      <c r="B94" s="6"/>
+      <c r="C94" s="2"/>
       <c r="E94" s="10"/>
     </row>
-    <row r="95" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E95" s="10"/>
     </row>
-    <row r="96" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E96" s="10"/>
     </row>
     <row r="97" spans="5:5" x14ac:dyDescent="0.25">
@@ -2268,22 +2838,55 @@
     <row r="230" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E230" s="10"/>
     </row>
-    <row r="1048576" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1048576" s="2"/>
+    <row r="231" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E231" s="10"/>
+    </row>
+    <row r="232" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E232" s="10"/>
+    </row>
+    <row r="233" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E233" s="10"/>
+    </row>
+    <row r="234" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E234" s="10"/>
+    </row>
+    <row r="235" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E235" s="10"/>
+    </row>
+    <row r="236" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E236" s="10"/>
+    </row>
+    <row r="237" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E237" s="10"/>
+    </row>
+    <row r="238" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E238" s="10"/>
+    </row>
+    <row r="239" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E239" s="10"/>
+    </row>
+    <row r="240" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E240" s="10"/>
+    </row>
+    <row r="241" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E241" s="10"/>
+    </row>
+    <row r="242" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E242" s="10"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E55" xr:uid="{2D001387-04E3-4955-8CAF-0DBBBF22CEAF}"/>
+  <autoFilter ref="A1:E67" xr:uid="{2D001387-04E3-4955-8CAF-0DBBBF22CEAF}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0627B16-E6A6-4FDA-A605-D8A29593EF93}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomLeft" activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2319,7 +2922,7 @@
         <v>44585</v>
       </c>
       <c r="B3" s="6">
-        <f t="shared" ref="B3:B13" si="0">B2+1</f>
+        <f t="shared" ref="B3:B16" si="0">B2+1</f>
         <v>219</v>
       </c>
       <c r="C3" s="9" t="s">
@@ -2328,7 +2931,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <f t="shared" ref="A4:A13" si="1">A3+1</f>
+        <f t="shared" ref="A4:A16" si="1">A3+1</f>
         <v>44586</v>
       </c>
       <c r="B4" s="6">
@@ -2454,6 +3057,45 @@
       </c>
       <c r="C13" s="9" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <f t="shared" si="1"/>
+        <v>44596</v>
+      </c>
+      <c r="B14" s="6">
+        <f t="shared" si="0"/>
+        <v>230</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <f t="shared" si="1"/>
+        <v>44597</v>
+      </c>
+      <c r="B15" s="6">
+        <f t="shared" si="0"/>
+        <v>231</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <f t="shared" si="1"/>
+        <v>44598</v>
+      </c>
+      <c r="B16" s="6">
+        <f t="shared" si="0"/>
+        <v>232</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed an issue on one of Erik's wordles
</commit_message>
<xml_diff>
--- a/Wordle Tracking.xlsx
+++ b/Wordle Tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riese\WordleTracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{305507D3-4739-43AC-99BC-493AE25F2409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA3689B-7B6B-43DF-8859-E627B82A7190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F705EBF7-AD41-4B67-999F-6C40503692F5}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Words" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Results!$A$1:$E$67</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Results!$A$1:$E$91</definedName>
     <definedName name="wordle_dates">OFFSET(Words!$A$2,,,COUNTA(Words!$A:$A)-1)</definedName>
     <definedName name="wordle_ids">OFFSET(Words!$B$2,,,COUNTA(Words!$B:$B)-1)</definedName>
     <definedName name="wordles">OFFSET(Words!$C$2,,,COUNTA(Words!$B:$B)-1)</definedName>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -542,7 +542,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
+      <selection pane="bottomLeft" activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1068,8 +1068,8 @@
         <f t="array" aca="1" ref="D27" ca="1">IF(_xlfn.XLOOKUP($B27,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B27,wordle_ids,wordles))</f>
         <v>MOUNT</v>
       </c>
-      <c r="E27" s="10" t="s">
-        <v>18</v>
+      <c r="E27" s="10">
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -2875,7 +2875,7 @@
       <c r="E242" s="10"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E67" xr:uid="{2D001387-04E3-4955-8CAF-0DBBBF22CEAF}"/>
+  <autoFilter ref="A1:E91" xr:uid="{2D001387-04E3-4955-8CAF-0DBBBF22CEAF}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Fixed an issue with the date column, added in 2/7/22 results and changed the color of one of the Wordle bar charts.
</commit_message>
<xml_diff>
--- a/Wordle Tracking.xlsx
+++ b/Wordle Tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rriesenb\Personal\Wordle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E103F02-D3A7-4574-9AC9-04DF735CD690}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9B1B60A-4728-4D7C-9768-0707E60E9CBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F705EBF7-AD41-4B67-999F-6C40503692F5}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>Date</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>PLEAT</t>
+  </si>
+  <si>
+    <t>ELDER</t>
   </si>
 </sst>
 </file>
@@ -542,7 +545,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,7 +573,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>44219</v>
+        <v>44584</v>
       </c>
       <c r="B2" s="4">
         <v>218</v>
@@ -588,7 +591,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <v>44219</v>
+        <v>44584</v>
       </c>
       <c r="B3" s="4">
         <v>218</v>
@@ -606,7 +609,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
-        <v>44219</v>
+        <v>44584</v>
       </c>
       <c r="B4" s="4">
         <v>218</v>
@@ -624,7 +627,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>44219</v>
+        <v>44584</v>
       </c>
       <c r="B5" s="4">
         <v>218</v>
@@ -640,7 +643,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
-        <v>44219</v>
+        <v>44584</v>
       </c>
       <c r="B6" s="4">
         <v>218</v>
@@ -656,7 +659,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
-        <v>44219</v>
+        <v>44584</v>
       </c>
       <c r="B7" s="4">
         <v>218</v>
@@ -673,7 +676,7 @@
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <f t="shared" ref="A8:A31" si="0">A2+1</f>
-        <v>44220</v>
+        <v>44585</v>
       </c>
       <c r="B8" s="6">
         <f t="shared" ref="B8:B31" si="1">B2+1</f>
@@ -694,7 +697,7 @@
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
-        <v>44220</v>
+        <v>44585</v>
       </c>
       <c r="B9" s="6">
         <f t="shared" si="1"/>
@@ -715,7 +718,7 @@
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
-        <v>44220</v>
+        <v>44585</v>
       </c>
       <c r="B10" s="6">
         <f t="shared" si="1"/>
@@ -736,7 +739,7 @@
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
-        <v>44220</v>
+        <v>44585</v>
       </c>
       <c r="B11" s="6">
         <f t="shared" si="1"/>
@@ -755,7 +758,7 @@
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <f t="shared" si="0"/>
-        <v>44220</v>
+        <v>44585</v>
       </c>
       <c r="B12" s="6">
         <f t="shared" si="1"/>
@@ -774,7 +777,7 @@
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
-        <v>44220</v>
+        <v>44585</v>
       </c>
       <c r="B13" s="6">
         <f t="shared" si="1"/>
@@ -793,7 +796,7 @@
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <f t="shared" si="0"/>
-        <v>44221</v>
+        <v>44586</v>
       </c>
       <c r="B14" s="6">
         <f t="shared" si="1"/>
@@ -814,7 +817,7 @@
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <f t="shared" si="0"/>
-        <v>44221</v>
+        <v>44586</v>
       </c>
       <c r="B15" s="6">
         <f t="shared" si="1"/>
@@ -835,7 +838,7 @@
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <f t="shared" si="0"/>
-        <v>44221</v>
+        <v>44586</v>
       </c>
       <c r="B16" s="6">
         <f t="shared" si="1"/>
@@ -856,7 +859,7 @@
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <f t="shared" si="0"/>
-        <v>44221</v>
+        <v>44586</v>
       </c>
       <c r="B17" s="6">
         <f t="shared" si="1"/>
@@ -875,7 +878,7 @@
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <f t="shared" si="0"/>
-        <v>44221</v>
+        <v>44586</v>
       </c>
       <c r="B18" s="6">
         <f t="shared" si="1"/>
@@ -894,7 +897,7 @@
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <f t="shared" si="0"/>
-        <v>44221</v>
+        <v>44586</v>
       </c>
       <c r="B19" s="6">
         <f t="shared" si="1"/>
@@ -913,7 +916,7 @@
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <f t="shared" si="0"/>
-        <v>44222</v>
+        <v>44587</v>
       </c>
       <c r="B20" s="6">
         <f t="shared" si="1"/>
@@ -934,7 +937,7 @@
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <f t="shared" si="0"/>
-        <v>44222</v>
+        <v>44587</v>
       </c>
       <c r="B21" s="6">
         <f t="shared" si="1"/>
@@ -955,7 +958,7 @@
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <f t="shared" si="0"/>
-        <v>44222</v>
+        <v>44587</v>
       </c>
       <c r="B22" s="6">
         <f t="shared" si="1"/>
@@ -976,7 +979,7 @@
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <f t="shared" si="0"/>
-        <v>44222</v>
+        <v>44587</v>
       </c>
       <c r="B23" s="6">
         <f t="shared" si="1"/>
@@ -995,7 +998,7 @@
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <f t="shared" si="0"/>
-        <v>44222</v>
+        <v>44587</v>
       </c>
       <c r="B24" s="6">
         <f t="shared" si="1"/>
@@ -1014,7 +1017,7 @@
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <f t="shared" si="0"/>
-        <v>44222</v>
+        <v>44587</v>
       </c>
       <c r="B25" s="6">
         <f t="shared" si="1"/>
@@ -1033,7 +1036,7 @@
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <f t="shared" si="0"/>
-        <v>44223</v>
+        <v>44588</v>
       </c>
       <c r="B26" s="6">
         <f t="shared" si="1"/>
@@ -1054,7 +1057,7 @@
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <f t="shared" si="0"/>
-        <v>44223</v>
+        <v>44588</v>
       </c>
       <c r="B27" s="6">
         <f t="shared" si="1"/>
@@ -1075,7 +1078,7 @@
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <f t="shared" si="0"/>
-        <v>44223</v>
+        <v>44588</v>
       </c>
       <c r="B28" s="6">
         <f t="shared" si="1"/>
@@ -1096,7 +1099,7 @@
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <f t="shared" si="0"/>
-        <v>44223</v>
+        <v>44588</v>
       </c>
       <c r="B29" s="6">
         <f t="shared" si="1"/>
@@ -1117,7 +1120,7 @@
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <f t="shared" si="0"/>
-        <v>44223</v>
+        <v>44588</v>
       </c>
       <c r="B30" s="6">
         <f t="shared" si="1"/>
@@ -1138,7 +1141,7 @@
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <f t="shared" si="0"/>
-        <v>44223</v>
+        <v>44588</v>
       </c>
       <c r="B31" s="6">
         <f t="shared" si="1"/>
@@ -1159,10 +1162,10 @@
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <f>A26+1</f>
-        <v>44224</v>
+        <v>44589</v>
       </c>
       <c r="B32" s="6">
-        <f t="shared" ref="B32:B91" si="3">B26+1</f>
+        <f t="shared" ref="B32:B97" si="3">B26+1</f>
         <v>223</v>
       </c>
       <c r="C32" s="2" t="str">
@@ -1179,15 +1182,15 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <f t="shared" ref="A33:A91" si="4">A27+1</f>
-        <v>44224</v>
+        <f t="shared" ref="A33:A97" si="4">A27+1</f>
+        <v>44589</v>
       </c>
       <c r="B33" s="6">
         <f t="shared" si="3"/>
         <v>223</v>
       </c>
       <c r="C33" s="2" t="str">
-        <f t="shared" ref="C33:C91" si="5">C27</f>
+        <f t="shared" ref="C33:C97" si="5">C27</f>
         <v>Erik</v>
       </c>
       <c r="D33" t="str" cm="1">
@@ -1201,7 +1204,7 @@
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <f t="shared" si="4"/>
-        <v>44224</v>
+        <v>44589</v>
       </c>
       <c r="B34" s="6">
         <f t="shared" si="3"/>
@@ -1222,7 +1225,7 @@
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <f t="shared" si="4"/>
-        <v>44224</v>
+        <v>44589</v>
       </c>
       <c r="B35" s="6">
         <f t="shared" si="3"/>
@@ -1243,7 +1246,7 @@
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <f t="shared" si="4"/>
-        <v>44224</v>
+        <v>44589</v>
       </c>
       <c r="B36" s="6">
         <f t="shared" si="3"/>
@@ -1264,7 +1267,7 @@
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <f t="shared" si="4"/>
-        <v>44224</v>
+        <v>44589</v>
       </c>
       <c r="B37" s="6">
         <f t="shared" si="3"/>
@@ -1285,7 +1288,7 @@
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <f t="shared" si="4"/>
-        <v>44225</v>
+        <v>44590</v>
       </c>
       <c r="B38" s="6">
         <f t="shared" si="3"/>
@@ -1306,7 +1309,7 @@
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <f t="shared" si="4"/>
-        <v>44225</v>
+        <v>44590</v>
       </c>
       <c r="B39" s="6">
         <f t="shared" si="3"/>
@@ -1327,7 +1330,7 @@
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <f t="shared" si="4"/>
-        <v>44225</v>
+        <v>44590</v>
       </c>
       <c r="B40" s="6">
         <f t="shared" si="3"/>
@@ -1348,7 +1351,7 @@
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <f t="shared" si="4"/>
-        <v>44225</v>
+        <v>44590</v>
       </c>
       <c r="B41" s="6">
         <f t="shared" si="3"/>
@@ -1369,7 +1372,7 @@
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <f t="shared" si="4"/>
-        <v>44225</v>
+        <v>44590</v>
       </c>
       <c r="B42" s="6">
         <f t="shared" si="3"/>
@@ -1390,7 +1393,7 @@
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <f t="shared" si="4"/>
-        <v>44225</v>
+        <v>44590</v>
       </c>
       <c r="B43" s="6">
         <f t="shared" si="3"/>
@@ -1409,7 +1412,7 @@
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <f t="shared" si="4"/>
-        <v>44226</v>
+        <v>44591</v>
       </c>
       <c r="B44" s="6">
         <f t="shared" si="3"/>
@@ -1430,7 +1433,7 @@
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <f t="shared" si="4"/>
-        <v>44226</v>
+        <v>44591</v>
       </c>
       <c r="B45" s="6">
         <f t="shared" si="3"/>
@@ -1451,7 +1454,7 @@
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <f t="shared" si="4"/>
-        <v>44226</v>
+        <v>44591</v>
       </c>
       <c r="B46" s="6">
         <f t="shared" si="3"/>
@@ -1472,7 +1475,7 @@
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <f t="shared" si="4"/>
-        <v>44226</v>
+        <v>44591</v>
       </c>
       <c r="B47" s="6">
         <f t="shared" si="3"/>
@@ -1493,7 +1496,7 @@
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <f t="shared" si="4"/>
-        <v>44226</v>
+        <v>44591</v>
       </c>
       <c r="B48" s="6">
         <f t="shared" si="3"/>
@@ -1514,7 +1517,7 @@
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <f t="shared" si="4"/>
-        <v>44226</v>
+        <v>44591</v>
       </c>
       <c r="B49" s="6">
         <f t="shared" si="3"/>
@@ -1533,7 +1536,7 @@
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <f t="shared" si="4"/>
-        <v>44227</v>
+        <v>44592</v>
       </c>
       <c r="B50" s="6">
         <f t="shared" si="3"/>
@@ -1554,7 +1557,7 @@
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <f t="shared" si="4"/>
-        <v>44227</v>
+        <v>44592</v>
       </c>
       <c r="B51" s="6">
         <f t="shared" si="3"/>
@@ -1575,7 +1578,7 @@
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <f t="shared" si="4"/>
-        <v>44227</v>
+        <v>44592</v>
       </c>
       <c r="B52" s="6">
         <f t="shared" si="3"/>
@@ -1596,7 +1599,7 @@
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <f t="shared" si="4"/>
-        <v>44227</v>
+        <v>44592</v>
       </c>
       <c r="B53" s="6">
         <f t="shared" si="3"/>
@@ -1617,7 +1620,7 @@
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <f t="shared" si="4"/>
-        <v>44227</v>
+        <v>44592</v>
       </c>
       <c r="B54" s="6">
         <f t="shared" si="3"/>
@@ -1638,7 +1641,7 @@
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <f>A49+1</f>
-        <v>44227</v>
+        <v>44592</v>
       </c>
       <c r="B55" s="6">
         <f t="shared" si="3"/>
@@ -1659,7 +1662,7 @@
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <f t="shared" si="4"/>
-        <v>44228</v>
+        <v>44593</v>
       </c>
       <c r="B56" s="6">
         <f t="shared" si="3"/>
@@ -1680,7 +1683,7 @@
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <f t="shared" si="4"/>
-        <v>44228</v>
+        <v>44593</v>
       </c>
       <c r="B57" s="6">
         <f t="shared" si="3"/>
@@ -1701,7 +1704,7 @@
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <f t="shared" si="4"/>
-        <v>44228</v>
+        <v>44593</v>
       </c>
       <c r="B58" s="6">
         <f t="shared" si="3"/>
@@ -1722,7 +1725,7 @@
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <f t="shared" si="4"/>
-        <v>44228</v>
+        <v>44593</v>
       </c>
       <c r="B59" s="6">
         <f t="shared" si="3"/>
@@ -1743,7 +1746,7 @@
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <f t="shared" si="4"/>
-        <v>44228</v>
+        <v>44593</v>
       </c>
       <c r="B60" s="6">
         <f t="shared" si="3"/>
@@ -1764,7 +1767,7 @@
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <f t="shared" si="4"/>
-        <v>44228</v>
+        <v>44593</v>
       </c>
       <c r="B61" s="6">
         <f t="shared" si="3"/>
@@ -1785,7 +1788,7 @@
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <f t="shared" si="4"/>
-        <v>44229</v>
+        <v>44594</v>
       </c>
       <c r="B62" s="6">
         <f t="shared" si="3"/>
@@ -1806,7 +1809,7 @@
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <f t="shared" si="4"/>
-        <v>44229</v>
+        <v>44594</v>
       </c>
       <c r="B63" s="6">
         <f t="shared" si="3"/>
@@ -1827,7 +1830,7 @@
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <f t="shared" si="4"/>
-        <v>44229</v>
+        <v>44594</v>
       </c>
       <c r="B64" s="6">
         <f t="shared" si="3"/>
@@ -1848,7 +1851,7 @@
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <f t="shared" si="4"/>
-        <v>44229</v>
+        <v>44594</v>
       </c>
       <c r="B65" s="6">
         <f t="shared" si="3"/>
@@ -1869,7 +1872,7 @@
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <f t="shared" si="4"/>
-        <v>44229</v>
+        <v>44594</v>
       </c>
       <c r="B66" s="6">
         <f t="shared" si="3"/>
@@ -1890,7 +1893,7 @@
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <f t="shared" si="4"/>
-        <v>44229</v>
+        <v>44594</v>
       </c>
       <c r="B67" s="6">
         <f t="shared" si="3"/>
@@ -1911,7 +1914,7 @@
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <f t="shared" si="4"/>
-        <v>44230</v>
+        <v>44595</v>
       </c>
       <c r="B68" s="6">
         <f t="shared" si="3"/>
@@ -1932,7 +1935,7 @@
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <f t="shared" si="4"/>
-        <v>44230</v>
+        <v>44595</v>
       </c>
       <c r="B69" s="6">
         <f t="shared" si="3"/>
@@ -1953,7 +1956,7 @@
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <f t="shared" si="4"/>
-        <v>44230</v>
+        <v>44595</v>
       </c>
       <c r="B70" s="6">
         <f t="shared" si="3"/>
@@ -1974,7 +1977,7 @@
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <f t="shared" si="4"/>
-        <v>44230</v>
+        <v>44595</v>
       </c>
       <c r="B71" s="6">
         <f t="shared" si="3"/>
@@ -1995,7 +1998,7 @@
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <f t="shared" si="4"/>
-        <v>44230</v>
+        <v>44595</v>
       </c>
       <c r="B72" s="6">
         <f t="shared" si="3"/>
@@ -2016,7 +2019,7 @@
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <f t="shared" si="4"/>
-        <v>44230</v>
+        <v>44595</v>
       </c>
       <c r="B73" s="6">
         <f t="shared" si="3"/>
@@ -2037,7 +2040,7 @@
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <f t="shared" si="4"/>
-        <v>44231</v>
+        <v>44596</v>
       </c>
       <c r="B74" s="6">
         <f t="shared" si="3"/>
@@ -2058,7 +2061,7 @@
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <f t="shared" si="4"/>
-        <v>44231</v>
+        <v>44596</v>
       </c>
       <c r="B75" s="6">
         <f t="shared" si="3"/>
@@ -2079,7 +2082,7 @@
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <f t="shared" si="4"/>
-        <v>44231</v>
+        <v>44596</v>
       </c>
       <c r="B76" s="6">
         <f t="shared" si="3"/>
@@ -2100,7 +2103,7 @@
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <f t="shared" si="4"/>
-        <v>44231</v>
+        <v>44596</v>
       </c>
       <c r="B77" s="6">
         <f t="shared" si="3"/>
@@ -2121,7 +2124,7 @@
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <f t="shared" si="4"/>
-        <v>44231</v>
+        <v>44596</v>
       </c>
       <c r="B78" s="6">
         <f t="shared" si="3"/>
@@ -2142,7 +2145,7 @@
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <f t="shared" si="4"/>
-        <v>44231</v>
+        <v>44596</v>
       </c>
       <c r="B79" s="6">
         <f t="shared" si="3"/>
@@ -2163,7 +2166,7 @@
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <f t="shared" si="4"/>
-        <v>44232</v>
+        <v>44597</v>
       </c>
       <c r="B80" s="6">
         <f t="shared" si="3"/>
@@ -2184,7 +2187,7 @@
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <f t="shared" si="4"/>
-        <v>44232</v>
+        <v>44597</v>
       </c>
       <c r="B81" s="6">
         <f t="shared" si="3"/>
@@ -2205,7 +2208,7 @@
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <f t="shared" si="4"/>
-        <v>44232</v>
+        <v>44597</v>
       </c>
       <c r="B82" s="6">
         <f t="shared" si="3"/>
@@ -2226,7 +2229,7 @@
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <f t="shared" si="4"/>
-        <v>44232</v>
+        <v>44597</v>
       </c>
       <c r="B83" s="6">
         <f t="shared" si="3"/>
@@ -2247,7 +2250,7 @@
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <f t="shared" si="4"/>
-        <v>44232</v>
+        <v>44597</v>
       </c>
       <c r="B84" s="6">
         <f t="shared" si="3"/>
@@ -2268,7 +2271,7 @@
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <f t="shared" si="4"/>
-        <v>44232</v>
+        <v>44597</v>
       </c>
       <c r="B85" s="6">
         <f t="shared" si="3"/>
@@ -2289,7 +2292,7 @@
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <f t="shared" si="4"/>
-        <v>44233</v>
+        <v>44598</v>
       </c>
       <c r="B86" s="6">
         <f t="shared" si="3"/>
@@ -2310,7 +2313,7 @@
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <f t="shared" si="4"/>
-        <v>44233</v>
+        <v>44598</v>
       </c>
       <c r="B87" s="6">
         <f t="shared" si="3"/>
@@ -2331,7 +2334,7 @@
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <f t="shared" si="4"/>
-        <v>44233</v>
+        <v>44598</v>
       </c>
       <c r="B88" s="6">
         <f t="shared" si="3"/>
@@ -2352,7 +2355,7 @@
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <f t="shared" si="4"/>
-        <v>44233</v>
+        <v>44598</v>
       </c>
       <c r="B89" s="6">
         <f t="shared" si="3"/>
@@ -2373,7 +2376,7 @@
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <f t="shared" si="4"/>
-        <v>44233</v>
+        <v>44598</v>
       </c>
       <c r="B90" s="6">
         <f t="shared" si="3"/>
@@ -2394,7 +2397,7 @@
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <f t="shared" si="4"/>
-        <v>44233</v>
+        <v>44598</v>
       </c>
       <c r="B91" s="6">
         <f t="shared" si="3"/>
@@ -2413,75 +2416,183 @@
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="2"/>
-      <c r="B92" s="6"/>
-      <c r="C92" s="2"/>
-      <c r="E92" s="10"/>
+      <c r="A92" s="2">
+        <f t="shared" si="4"/>
+        <v>44599</v>
+      </c>
+      <c r="B92" s="6">
+        <f t="shared" si="3"/>
+        <v>233</v>
+      </c>
+      <c r="C92" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>Phil</v>
+      </c>
+      <c r="D92" t="str" cm="1">
+        <f t="array" aca="1" ref="D92" ca="1">IF(_xlfn.XLOOKUP($B92,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B92,wordle_ids,wordles))</f>
+        <v>ELDER</v>
+      </c>
+      <c r="E92" s="10">
+        <v>6</v>
+      </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" s="2"/>
-      <c r="B93" s="6"/>
-      <c r="C93" s="2"/>
-      <c r="E93" s="10"/>
+      <c r="A93" s="2">
+        <f t="shared" si="4"/>
+        <v>44599</v>
+      </c>
+      <c r="B93" s="6">
+        <f t="shared" si="3"/>
+        <v>233</v>
+      </c>
+      <c r="C93" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>Erik</v>
+      </c>
+      <c r="D93" t="str" cm="1">
+        <f t="array" aca="1" ref="D93" ca="1">IF(_xlfn.XLOOKUP($B93,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B93,wordle_ids,wordles))</f>
+        <v>ELDER</v>
+      </c>
+      <c r="E93" s="10">
+        <v>5</v>
+      </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" s="2"/>
-      <c r="B94" s="6"/>
-      <c r="C94" s="2"/>
-      <c r="E94" s="10"/>
+      <c r="A94" s="2">
+        <f t="shared" si="4"/>
+        <v>44599</v>
+      </c>
+      <c r="B94" s="6">
+        <f t="shared" si="3"/>
+        <v>233</v>
+      </c>
+      <c r="C94" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>RoBert</v>
+      </c>
+      <c r="D94" t="str" cm="1">
+        <f t="array" aca="1" ref="D94" ca="1">IF(_xlfn.XLOOKUP($B94,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B94,wordle_ids,wordles))</f>
+        <v>ELDER</v>
+      </c>
+      <c r="E94" s="10">
+        <v>4</v>
+      </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E95" s="10"/>
+      <c r="A95" s="2">
+        <f t="shared" si="4"/>
+        <v>44599</v>
+      </c>
+      <c r="B95" s="6">
+        <f t="shared" si="3"/>
+        <v>233</v>
+      </c>
+      <c r="C95" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>Andrew</v>
+      </c>
+      <c r="D95" t="str" cm="1">
+        <f t="array" aca="1" ref="D95" ca="1">IF(_xlfn.XLOOKUP($B95,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B95,wordle_ids,wordles))</f>
+        <v>ELDER</v>
+      </c>
+      <c r="E95" s="10">
+        <v>4</v>
+      </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E96" s="10"/>
-    </row>
-    <row r="97" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E97" s="10"/>
-    </row>
-    <row r="98" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="2">
+        <f t="shared" si="4"/>
+        <v>44599</v>
+      </c>
+      <c r="B96" s="6">
+        <f t="shared" si="3"/>
+        <v>233</v>
+      </c>
+      <c r="C96" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>Yoyo</v>
+      </c>
+      <c r="D96" t="str" cm="1">
+        <f t="array" aca="1" ref="D96" ca="1">IF(_xlfn.XLOOKUP($B96,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B96,wordle_ids,wordles))</f>
+        <v>ELDER</v>
+      </c>
+      <c r="E96" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="2">
+        <f t="shared" si="4"/>
+        <v>44599</v>
+      </c>
+      <c r="B97" s="6">
+        <f t="shared" si="3"/>
+        <v>233</v>
+      </c>
+      <c r="C97" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>Henry</v>
+      </c>
+      <c r="D97" t="str" cm="1">
+        <f t="array" aca="1" ref="D97" ca="1">IF(_xlfn.XLOOKUP($B97,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B97,wordle_ids,wordles))</f>
+        <v>ELDER</v>
+      </c>
+      <c r="E97" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" s="2"/>
+      <c r="B98" s="6"/>
+      <c r="C98" s="2"/>
       <c r="E98" s="10"/>
     </row>
-    <row r="99" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="2"/>
+      <c r="B99" s="6"/>
+      <c r="C99" s="2"/>
       <c r="E99" s="10"/>
     </row>
-    <row r="100" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" s="2"/>
+      <c r="B100" s="6"/>
+      <c r="C100" s="2"/>
       <c r="E100" s="10"/>
     </row>
-    <row r="101" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E101" s="10"/>
     </row>
-    <row r="102" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E102" s="10"/>
     </row>
-    <row r="103" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E103" s="10"/>
     </row>
-    <row r="104" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E104" s="10"/>
     </row>
-    <row r="105" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E105" s="10"/>
     </row>
-    <row r="106" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E106" s="10"/>
     </row>
-    <row r="107" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E107" s="10"/>
     </row>
-    <row r="108" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E108" s="10"/>
     </row>
-    <row r="109" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E109" s="10"/>
     </row>
-    <row r="110" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E110" s="10"/>
     </row>
-    <row r="111" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E111" s="10"/>
     </row>
-    <row r="112" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E112" s="10"/>
     </row>
     <row r="113" spans="5:5" x14ac:dyDescent="0.25">
@@ -2882,11 +2993,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0627B16-E6A6-4FDA-A605-D8A29593EF93}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B36" sqref="B36"/>
+      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2922,7 +3033,7 @@
         <v>44585</v>
       </c>
       <c r="B3" s="6">
-        <f t="shared" ref="B3:B16" si="0">B2+1</f>
+        <f t="shared" ref="B3:B17" si="0">B2+1</f>
         <v>219</v>
       </c>
       <c r="C3" s="9" t="s">
@@ -2931,7 +3042,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <f t="shared" ref="A4:A16" si="1">A3+1</f>
+        <f t="shared" ref="A4:A17" si="1">A3+1</f>
         <v>44586</v>
       </c>
       <c r="B4" s="6">
@@ -3096,6 +3207,19 @@
       </c>
       <c r="C16" s="9" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <f t="shared" si="1"/>
+        <v>44599</v>
+      </c>
+      <c r="B17" s="6">
+        <f t="shared" si="0"/>
+        <v>233</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a Wordle History page & Aimee data
</commit_message>
<xml_diff>
--- a/Wordle Tracking.xlsx
+++ b/Wordle Tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riese\WordleTracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA3689B-7B6B-43DF-8859-E627B82A7190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B39E551-0623-4C8D-BDE8-C24F86D04B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F705EBF7-AD41-4B67-999F-6C40503692F5}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Words" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Results!$A$1:$E$91</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Results!$A$1:$E$113</definedName>
     <definedName name="wordle_dates">OFFSET(Words!$A$2,,,COUNTA(Words!$A:$A)-1)</definedName>
     <definedName name="wordle_ids">OFFSET(Words!$B$2,,,COUNTA(Words!$B:$B)-1)</definedName>
     <definedName name="wordles">OFFSET(Words!$C$2,,,COUNTA(Words!$B:$B)-1)</definedName>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>Date</t>
   </si>
@@ -147,6 +147,12 @@
   </si>
   <si>
     <t>PLEAT</t>
+  </si>
+  <si>
+    <t>ELDER</t>
+  </si>
+  <si>
+    <t>Aimee</t>
   </si>
 </sst>
 </file>
@@ -538,11 +544,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D001387-04E3-4955-8CAF-0DBBBF22CEAF}">
-  <dimension ref="A1:E242"/>
+  <dimension ref="A1:E257"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E33" sqref="E33"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,45 +677,40 @@
       <c r="E7" s="10"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <f t="shared" ref="A8:A31" si="0">A2+1</f>
-        <v>44220</v>
-      </c>
-      <c r="B8" s="6">
-        <f t="shared" ref="B8:B31" si="1">B2+1</f>
-        <v>219</v>
-      </c>
-      <c r="C8" s="2" t="str">
-        <f>C2</f>
-        <v>Phil</v>
+      <c r="A8" s="3">
+        <v>44219</v>
+      </c>
+      <c r="B8" s="4">
+        <v>218</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="D8" t="str" cm="1">
         <f t="array" aca="1" ref="D8" ca="1">IF(_xlfn.XLOOKUP($B8,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B8,wordle_ids,wordles))</f>
-        <v>KNOLL</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>18</v>
-      </c>
+        <v>CRIMP</v>
+      </c>
+      <c r="E8" s="10"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
+        <f t="shared" ref="A9:B15" si="0">A2+1</f>
+        <v>44220</v>
+      </c>
+      <c r="B9" s="6">
         <f t="shared" si="0"/>
-        <v>44220</v>
-      </c>
-      <c r="B9" s="6">
-        <f t="shared" si="1"/>
         <v>219</v>
       </c>
       <c r="C9" s="2" t="str">
-        <f t="shared" ref="C9:C31" si="2">C3</f>
-        <v>Erik</v>
+        <f t="shared" ref="C9:C15" si="1">C2</f>
+        <v>Phil</v>
       </c>
       <c r="D9" t="str" cm="1">
         <f t="array" aca="1" ref="D9" ca="1">IF(_xlfn.XLOOKUP($B9,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B9,wordle_ids,wordles))</f>
         <v>KNOLL</v>
       </c>
-      <c r="E9" s="10">
-        <v>5</v>
+      <c r="E9" s="10" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -718,12 +719,12 @@
         <v>44220</v>
       </c>
       <c r="B10" s="6">
+        <f t="shared" si="0"/>
+        <v>219</v>
+      </c>
+      <c r="C10" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>219</v>
-      </c>
-      <c r="C10" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>RoBert</v>
+        <v>Erik</v>
       </c>
       <c r="D10" t="str" cm="1">
         <f t="array" aca="1" ref="D10" ca="1">IF(_xlfn.XLOOKUP($B10,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B10,wordle_ids,wordles))</f>
@@ -739,18 +740,20 @@
         <v>44220</v>
       </c>
       <c r="B11" s="6">
+        <f t="shared" si="0"/>
+        <v>219</v>
+      </c>
+      <c r="C11" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>219</v>
-      </c>
-      <c r="C11" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>Andrew</v>
+        <v>RoBert</v>
       </c>
       <c r="D11" t="str" cm="1">
         <f t="array" aca="1" ref="D11" ca="1">IF(_xlfn.XLOOKUP($B11,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B11,wordle_ids,wordles))</f>
         <v>KNOLL</v>
       </c>
-      <c r="E11" s="10"/>
+      <c r="E11" s="10">
+        <v>5</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
@@ -758,12 +761,12 @@
         <v>44220</v>
       </c>
       <c r="B12" s="6">
+        <f t="shared" si="0"/>
+        <v>219</v>
+      </c>
+      <c r="C12" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>219</v>
-      </c>
-      <c r="C12" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>Yoyo</v>
+        <v>Andrew</v>
       </c>
       <c r="D12" t="str" cm="1">
         <f t="array" aca="1" ref="D12" ca="1">IF(_xlfn.XLOOKUP($B12,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B12,wordle_ids,wordles))</f>
@@ -777,12 +780,12 @@
         <v>44220</v>
       </c>
       <c r="B13" s="6">
+        <f t="shared" si="0"/>
+        <v>219</v>
+      </c>
+      <c r="C13" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>219</v>
-      </c>
-      <c r="C13" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>Henry</v>
+        <v>Yoyo</v>
       </c>
       <c r="D13" t="str" cm="1">
         <f t="array" aca="1" ref="D13" ca="1">IF(_xlfn.XLOOKUP($B13,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B13,wordle_ids,wordles))</f>
@@ -793,57 +796,53 @@
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <f t="shared" si="0"/>
-        <v>44221</v>
+        <v>44220</v>
       </c>
       <c r="B14" s="6">
+        <f t="shared" si="0"/>
+        <v>219</v>
+      </c>
+      <c r="C14" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>220</v>
-      </c>
-      <c r="C14" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>Phil</v>
+        <v>Henry</v>
       </c>
       <c r="D14" t="str" cm="1">
         <f t="array" aca="1" ref="D14" ca="1">IF(_xlfn.XLOOKUP($B14,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B14,wordle_ids,wordles))</f>
-        <v>SUGAR</v>
-      </c>
-      <c r="E14" s="10">
-        <v>4</v>
-      </c>
+        <v>KNOLL</v>
+      </c>
+      <c r="E14" s="10"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <f t="shared" si="0"/>
-        <v>44221</v>
+        <v>44220</v>
       </c>
       <c r="B15" s="6">
+        <f t="shared" si="0"/>
+        <v>219</v>
+      </c>
+      <c r="C15" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>220</v>
-      </c>
-      <c r="C15" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>Erik</v>
+        <v>Aimee</v>
       </c>
       <c r="D15" t="str" cm="1">
         <f t="array" aca="1" ref="D15" ca="1">IF(_xlfn.XLOOKUP($B15,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B15,wordle_ids,wordles))</f>
-        <v>SUGAR</v>
-      </c>
-      <c r="E15" s="10">
-        <v>3</v>
-      </c>
+        <v>KNOLL</v>
+      </c>
+      <c r="E15" s="10"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="A16:B16" si="2">A9+1</f>
         <v>44221</v>
       </c>
       <c r="B16" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>220</v>
       </c>
       <c r="C16" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>RoBert</v>
+        <f t="shared" ref="C16:C113" si="3">C9</f>
+        <v>Phil</v>
       </c>
       <c r="D16" t="str" cm="1">
         <f t="array" aca="1" ref="D16" ca="1">IF(_xlfn.XLOOKUP($B16,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B16,wordle_ids,wordles))</f>
@@ -855,54 +854,58 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="A17:B17" si="4">A10+1</f>
         <v>44221</v>
       </c>
       <c r="B17" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>220</v>
       </c>
       <c r="C17" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>Andrew</v>
+        <f t="shared" si="3"/>
+        <v>Erik</v>
       </c>
       <c r="D17" t="str" cm="1">
         <f t="array" aca="1" ref="D17" ca="1">IF(_xlfn.XLOOKUP($B17,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B17,wordle_ids,wordles))</f>
         <v>SUGAR</v>
       </c>
-      <c r="E17" s="10"/>
+      <c r="E17" s="10">
+        <v>3</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="A18:B18" si="5">A11+1</f>
         <v>44221</v>
       </c>
       <c r="B18" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>220</v>
       </c>
       <c r="C18" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>Yoyo</v>
+        <f t="shared" si="3"/>
+        <v>RoBert</v>
       </c>
       <c r="D18" t="str" cm="1">
         <f t="array" aca="1" ref="D18" ca="1">IF(_xlfn.XLOOKUP($B18,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B18,wordle_ids,wordles))</f>
         <v>SUGAR</v>
       </c>
-      <c r="E18" s="10"/>
+      <c r="E18" s="10">
+        <v>4</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="A19:B19" si="6">A12+1</f>
         <v>44221</v>
       </c>
       <c r="B19" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>220</v>
       </c>
       <c r="C19" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>Henry</v>
+        <f t="shared" si="3"/>
+        <v>Andrew</v>
       </c>
       <c r="D19" t="str" cm="1">
         <f t="array" aca="1" ref="D19" ca="1">IF(_xlfn.XLOOKUP($B19,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B19,wordle_ids,wordles))</f>
@@ -912,241 +915,233 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <f t="shared" si="0"/>
-        <v>44222</v>
+        <f t="shared" ref="A20:B20" si="7">A13+1</f>
+        <v>44221</v>
       </c>
       <c r="B20" s="6">
-        <f t="shared" si="1"/>
-        <v>221</v>
+        <f t="shared" si="7"/>
+        <v>220</v>
       </c>
       <c r="C20" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>Phil</v>
+        <f t="shared" si="3"/>
+        <v>Yoyo</v>
       </c>
       <c r="D20" t="str" cm="1">
         <f t="array" aca="1" ref="D20" ca="1">IF(_xlfn.XLOOKUP($B20,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B20,wordle_ids,wordles))</f>
-        <v>WHACK</v>
-      </c>
-      <c r="E20" s="10">
-        <v>4</v>
-      </c>
+        <v>SUGAR</v>
+      </c>
+      <c r="E20" s="10"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <f t="shared" si="0"/>
-        <v>44222</v>
+        <f t="shared" ref="A21:B21" si="8">A14+1</f>
+        <v>44221</v>
       </c>
       <c r="B21" s="6">
-        <f t="shared" si="1"/>
-        <v>221</v>
+        <f t="shared" si="8"/>
+        <v>220</v>
       </c>
       <c r="C21" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>Erik</v>
+        <f t="shared" si="3"/>
+        <v>Henry</v>
       </c>
       <c r="D21" t="str" cm="1">
         <f t="array" aca="1" ref="D21" ca="1">IF(_xlfn.XLOOKUP($B21,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B21,wordle_ids,wordles))</f>
-        <v>WHACK</v>
-      </c>
-      <c r="E21" s="10">
-        <v>5</v>
-      </c>
+        <v>SUGAR</v>
+      </c>
+      <c r="E21" s="10"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <f t="shared" si="0"/>
-        <v>44222</v>
+        <f t="shared" ref="A22:B22" si="9">A15+1</f>
+        <v>44221</v>
       </c>
       <c r="B22" s="6">
-        <f t="shared" si="1"/>
-        <v>221</v>
+        <f t="shared" si="9"/>
+        <v>220</v>
       </c>
       <c r="C22" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>RoBert</v>
+        <f t="shared" si="3"/>
+        <v>Aimee</v>
       </c>
       <c r="D22" t="str" cm="1">
         <f t="array" aca="1" ref="D22" ca="1">IF(_xlfn.XLOOKUP($B22,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B22,wordle_ids,wordles))</f>
-        <v>WHACK</v>
-      </c>
-      <c r="E22" s="10">
-        <v>4</v>
-      </c>
+        <v>SUGAR</v>
+      </c>
+      <c r="E22" s="10"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="A23:B23" si="10">A16+1</f>
         <v>44222</v>
       </c>
       <c r="B23" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>221</v>
       </c>
       <c r="C23" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>Andrew</v>
+        <f t="shared" si="3"/>
+        <v>Phil</v>
       </c>
       <c r="D23" t="str" cm="1">
         <f t="array" aca="1" ref="D23" ca="1">IF(_xlfn.XLOOKUP($B23,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B23,wordle_ids,wordles))</f>
         <v>WHACK</v>
       </c>
-      <c r="E23" s="10"/>
+      <c r="E23" s="10">
+        <v>4</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="A24:B24" si="11">A17+1</f>
         <v>44222</v>
       </c>
       <c r="B24" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="11"/>
         <v>221</v>
       </c>
       <c r="C24" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>Yoyo</v>
+        <f t="shared" si="3"/>
+        <v>Erik</v>
       </c>
       <c r="D24" t="str" cm="1">
         <f t="array" aca="1" ref="D24" ca="1">IF(_xlfn.XLOOKUP($B24,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B24,wordle_ids,wordles))</f>
         <v>WHACK</v>
       </c>
-      <c r="E24" s="10"/>
+      <c r="E24" s="10">
+        <v>5</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="A25:B25" si="12">A18+1</f>
         <v>44222</v>
       </c>
       <c r="B25" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="12"/>
         <v>221</v>
       </c>
       <c r="C25" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>Henry</v>
+        <f t="shared" si="3"/>
+        <v>RoBert</v>
       </c>
       <c r="D25" t="str" cm="1">
         <f t="array" aca="1" ref="D25" ca="1">IF(_xlfn.XLOOKUP($B25,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B25,wordle_ids,wordles))</f>
         <v>WHACK</v>
       </c>
-      <c r="E25" s="10"/>
+      <c r="E25" s="10">
+        <v>4</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <f t="shared" si="0"/>
-        <v>44223</v>
+        <f t="shared" ref="A26:B26" si="13">A19+1</f>
+        <v>44222</v>
       </c>
       <c r="B26" s="6">
-        <f t="shared" si="1"/>
-        <v>222</v>
+        <f t="shared" si="13"/>
+        <v>221</v>
       </c>
       <c r="C26" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>Phil</v>
+        <f t="shared" si="3"/>
+        <v>Andrew</v>
       </c>
       <c r="D26" t="str" cm="1">
         <f t="array" aca="1" ref="D26" ca="1">IF(_xlfn.XLOOKUP($B26,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B26,wordle_ids,wordles))</f>
-        <v>MOUNT</v>
-      </c>
-      <c r="E26" s="10">
-        <v>3</v>
-      </c>
+        <v>WHACK</v>
+      </c>
+      <c r="E26" s="10"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <f t="shared" si="0"/>
-        <v>44223</v>
+        <f t="shared" ref="A27:B27" si="14">A20+1</f>
+        <v>44222</v>
       </c>
       <c r="B27" s="6">
-        <f t="shared" si="1"/>
-        <v>222</v>
+        <f t="shared" si="14"/>
+        <v>221</v>
       </c>
       <c r="C27" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>Erik</v>
+        <f t="shared" si="3"/>
+        <v>Yoyo</v>
       </c>
       <c r="D27" t="str" cm="1">
         <f t="array" aca="1" ref="D27" ca="1">IF(_xlfn.XLOOKUP($B27,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B27,wordle_ids,wordles))</f>
-        <v>MOUNT</v>
-      </c>
-      <c r="E27" s="10">
-        <v>5</v>
-      </c>
+        <v>WHACK</v>
+      </c>
+      <c r="E27" s="10"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <f t="shared" si="0"/>
-        <v>44223</v>
+        <f t="shared" ref="A28:B28" si="15">A21+1</f>
+        <v>44222</v>
       </c>
       <c r="B28" s="6">
-        <f t="shared" si="1"/>
-        <v>222</v>
+        <f t="shared" si="15"/>
+        <v>221</v>
       </c>
       <c r="C28" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>RoBert</v>
+        <f t="shared" si="3"/>
+        <v>Henry</v>
       </c>
       <c r="D28" t="str" cm="1">
         <f t="array" aca="1" ref="D28" ca="1">IF(_xlfn.XLOOKUP($B28,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B28,wordle_ids,wordles))</f>
-        <v>MOUNT</v>
-      </c>
-      <c r="E28" s="10">
-        <v>2</v>
-      </c>
+        <v>WHACK</v>
+      </c>
+      <c r="E28" s="10"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <f t="shared" si="0"/>
-        <v>44223</v>
+        <f t="shared" ref="A29:B29" si="16">A22+1</f>
+        <v>44222</v>
       </c>
       <c r="B29" s="6">
-        <f t="shared" si="1"/>
-        <v>222</v>
+        <f t="shared" si="16"/>
+        <v>221</v>
       </c>
       <c r="C29" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>Andrew</v>
+        <f t="shared" si="3"/>
+        <v>Aimee</v>
       </c>
       <c r="D29" t="str" cm="1">
         <f t="array" aca="1" ref="D29" ca="1">IF(_xlfn.XLOOKUP($B29,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B29,wordle_ids,wordles))</f>
-        <v>MOUNT</v>
-      </c>
-      <c r="E29" s="10">
-        <v>3</v>
-      </c>
+        <v>WHACK</v>
+      </c>
+      <c r="E29" s="10"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="A30:B30" si="17">A23+1</f>
         <v>44223</v>
       </c>
       <c r="B30" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="17"/>
         <v>222</v>
       </c>
       <c r="C30" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>Yoyo</v>
+        <f t="shared" si="3"/>
+        <v>Phil</v>
       </c>
       <c r="D30" t="str" cm="1">
         <f t="array" aca="1" ref="D30" ca="1">IF(_xlfn.XLOOKUP($B30,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B30,wordle_ids,wordles))</f>
         <v>MOUNT</v>
       </c>
       <c r="E30" s="10">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="A31:B31" si="18">A24+1</f>
         <v>44223</v>
       </c>
       <c r="B31" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="18"/>
         <v>222</v>
       </c>
       <c r="C31" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>Henry</v>
+        <f t="shared" si="3"/>
+        <v>Erik</v>
       </c>
       <c r="D31" t="str" cm="1">
         <f t="array" aca="1" ref="D31" ca="1">IF(_xlfn.XLOOKUP($B31,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B31,wordle_ids,wordles))</f>
@@ -1158,167 +1153,165 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <f>A26+1</f>
-        <v>44224</v>
+        <f t="shared" ref="A32:B32" si="19">A25+1</f>
+        <v>44223</v>
       </c>
       <c r="B32" s="6">
-        <f t="shared" ref="B32:B91" si="3">B26+1</f>
-        <v>223</v>
+        <f t="shared" si="19"/>
+        <v>222</v>
       </c>
       <c r="C32" s="2" t="str">
-        <f>C26</f>
-        <v>Phil</v>
+        <f t="shared" si="3"/>
+        <v>RoBert</v>
       </c>
       <c r="D32" t="str" cm="1">
         <f t="array" aca="1" ref="D32" ca="1">IF(_xlfn.XLOOKUP($B32,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B32,wordle_ids,wordles))</f>
-        <v>PERKY</v>
+        <v>MOUNT</v>
       </c>
       <c r="E32" s="10">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <f t="shared" ref="A33:A91" si="4">A27+1</f>
-        <v>44224</v>
+        <f t="shared" ref="A33:B33" si="20">A26+1</f>
+        <v>44223</v>
       </c>
       <c r="B33" s="6">
-        <f t="shared" si="3"/>
-        <v>223</v>
+        <f t="shared" si="20"/>
+        <v>222</v>
       </c>
       <c r="C33" s="2" t="str">
-        <f t="shared" ref="C33:C91" si="5">C27</f>
-        <v>Erik</v>
+        <f t="shared" si="3"/>
+        <v>Andrew</v>
       </c>
       <c r="D33" t="str" cm="1">
         <f t="array" aca="1" ref="D33" ca="1">IF(_xlfn.XLOOKUP($B33,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B33,wordle_ids,wordles))</f>
-        <v>PERKY</v>
+        <v>MOUNT</v>
       </c>
       <c r="E33" s="10">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <f t="shared" si="4"/>
-        <v>44224</v>
+        <f t="shared" ref="A34:B34" si="21">A27+1</f>
+        <v>44223</v>
       </c>
       <c r="B34" s="6">
-        <f t="shared" si="3"/>
-        <v>223</v>
+        <f t="shared" si="21"/>
+        <v>222</v>
       </c>
       <c r="C34" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>RoBert</v>
+        <f t="shared" si="3"/>
+        <v>Yoyo</v>
       </c>
       <c r="D34" t="str" cm="1">
         <f t="array" aca="1" ref="D34" ca="1">IF(_xlfn.XLOOKUP($B34,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B34,wordle_ids,wordles))</f>
-        <v>PERKY</v>
+        <v>MOUNT</v>
       </c>
       <c r="E34" s="10">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
-        <f t="shared" si="4"/>
-        <v>44224</v>
+        <f t="shared" ref="A35:B35" si="22">A28+1</f>
+        <v>44223</v>
       </c>
       <c r="B35" s="6">
-        <f t="shared" si="3"/>
-        <v>223</v>
+        <f t="shared" si="22"/>
+        <v>222</v>
       </c>
       <c r="C35" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Andrew</v>
+        <f t="shared" si="3"/>
+        <v>Henry</v>
       </c>
       <c r="D35" t="str" cm="1">
         <f t="array" aca="1" ref="D35" ca="1">IF(_xlfn.XLOOKUP($B35,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B35,wordle_ids,wordles))</f>
-        <v>PERKY</v>
-      </c>
-      <c r="E35" s="10" t="s">
-        <v>18</v>
+        <v>MOUNT</v>
+      </c>
+      <c r="E35" s="10">
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
-        <f t="shared" si="4"/>
-        <v>44224</v>
+        <f t="shared" ref="A36:B36" si="23">A29+1</f>
+        <v>44223</v>
       </c>
       <c r="B36" s="6">
-        <f t="shared" si="3"/>
-        <v>223</v>
+        <f t="shared" si="23"/>
+        <v>222</v>
       </c>
       <c r="C36" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Yoyo</v>
+        <f t="shared" si="3"/>
+        <v>Aimee</v>
       </c>
       <c r="D36" t="str" cm="1">
         <f t="array" aca="1" ref="D36" ca="1">IF(_xlfn.XLOOKUP($B36,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B36,wordle_ids,wordles))</f>
-        <v>PERKY</v>
-      </c>
-      <c r="E36" s="10">
-        <v>4</v>
-      </c>
+        <v>MOUNT</v>
+      </c>
+      <c r="E36" s="10"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="A37:B37" si="24">A30+1</f>
         <v>44224</v>
       </c>
       <c r="B37" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="24"/>
         <v>223</v>
       </c>
       <c r="C37" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Henry</v>
+        <f t="shared" si="3"/>
+        <v>Phil</v>
       </c>
       <c r="D37" t="str" cm="1">
         <f t="array" aca="1" ref="D37" ca="1">IF(_xlfn.XLOOKUP($B37,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B37,wordle_ids,wordles))</f>
         <v>PERKY</v>
       </c>
-      <c r="E37" s="10" t="s">
-        <v>18</v>
+      <c r="E37" s="10">
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
-        <f t="shared" si="4"/>
-        <v>44225</v>
+        <f t="shared" ref="A38:B38" si="25">A31+1</f>
+        <v>44224</v>
       </c>
       <c r="B38" s="6">
-        <f t="shared" si="3"/>
-        <v>224</v>
+        <f t="shared" si="25"/>
+        <v>223</v>
       </c>
       <c r="C38" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Phil</v>
+        <f t="shared" si="3"/>
+        <v>Erik</v>
       </c>
       <c r="D38" t="str" cm="1">
         <f t="array" aca="1" ref="D38" ca="1">IF(_xlfn.XLOOKUP($B38,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B38,wordle_ids,wordles))</f>
-        <v>COULD</v>
+        <v>PERKY</v>
       </c>
       <c r="E38" s="10">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
-        <f t="shared" si="4"/>
-        <v>44225</v>
+        <f t="shared" ref="A39:B39" si="26">A32+1</f>
+        <v>44224</v>
       </c>
       <c r="B39" s="6">
-        <f t="shared" si="3"/>
-        <v>224</v>
+        <f t="shared" si="26"/>
+        <v>223</v>
       </c>
       <c r="C39" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Erik</v>
+        <f t="shared" si="3"/>
+        <v>RoBert</v>
       </c>
       <c r="D39" t="str" cm="1">
         <f t="array" aca="1" ref="D39" ca="1">IF(_xlfn.XLOOKUP($B39,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B39,wordle_ids,wordles))</f>
-        <v>COULD</v>
+        <v>PERKY</v>
       </c>
       <c r="E39" s="10">
         <v>4</v>
@@ -1326,123 +1319,123 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
-        <f t="shared" si="4"/>
-        <v>44225</v>
+        <f t="shared" ref="A40:B40" si="27">A33+1</f>
+        <v>44224</v>
       </c>
       <c r="B40" s="6">
-        <f t="shared" si="3"/>
-        <v>224</v>
+        <f t="shared" si="27"/>
+        <v>223</v>
       </c>
       <c r="C40" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>RoBert</v>
+        <f t="shared" si="3"/>
+        <v>Andrew</v>
       </c>
       <c r="D40" t="str" cm="1">
         <f t="array" aca="1" ref="D40" ca="1">IF(_xlfn.XLOOKUP($B40,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B40,wordle_ids,wordles))</f>
-        <v>COULD</v>
-      </c>
-      <c r="E40" s="10">
-        <v>5</v>
+        <v>PERKY</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
-        <f t="shared" si="4"/>
-        <v>44225</v>
+        <f t="shared" ref="A41:B41" si="28">A34+1</f>
+        <v>44224</v>
       </c>
       <c r="B41" s="6">
-        <f t="shared" si="3"/>
-        <v>224</v>
+        <f t="shared" si="28"/>
+        <v>223</v>
       </c>
       <c r="C41" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Andrew</v>
+        <f t="shared" si="3"/>
+        <v>Yoyo</v>
       </c>
       <c r="D41" t="str" cm="1">
         <f t="array" aca="1" ref="D41" ca="1">IF(_xlfn.XLOOKUP($B41,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B41,wordle_ids,wordles))</f>
-        <v>COULD</v>
+        <v>PERKY</v>
       </c>
       <c r="E41" s="10">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
-        <f t="shared" si="4"/>
-        <v>44225</v>
+        <f t="shared" ref="A42:B42" si="29">A35+1</f>
+        <v>44224</v>
       </c>
       <c r="B42" s="6">
-        <f t="shared" si="3"/>
-        <v>224</v>
+        <f t="shared" si="29"/>
+        <v>223</v>
       </c>
       <c r="C42" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Yoyo</v>
+        <f t="shared" si="3"/>
+        <v>Henry</v>
       </c>
       <c r="D42" t="str" cm="1">
         <f t="array" aca="1" ref="D42" ca="1">IF(_xlfn.XLOOKUP($B42,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B42,wordle_ids,wordles))</f>
-        <v>COULD</v>
-      </c>
-      <c r="E42" s="10">
-        <v>4</v>
+        <v>PERKY</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
-        <f t="shared" si="4"/>
-        <v>44225</v>
+        <f t="shared" ref="A43:B43" si="30">A36+1</f>
+        <v>44224</v>
       </c>
       <c r="B43" s="6">
-        <f t="shared" si="3"/>
-        <v>224</v>
+        <f t="shared" si="30"/>
+        <v>223</v>
       </c>
       <c r="C43" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Henry</v>
+        <f t="shared" si="3"/>
+        <v>Aimee</v>
       </c>
       <c r="D43" t="str" cm="1">
         <f t="array" aca="1" ref="D43" ca="1">IF(_xlfn.XLOOKUP($B43,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B43,wordle_ids,wordles))</f>
-        <v>COULD</v>
+        <v>PERKY</v>
       </c>
       <c r="E43" s="10"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
-        <f t="shared" si="4"/>
-        <v>44226</v>
+        <f t="shared" ref="A44:B44" si="31">A37+1</f>
+        <v>44225</v>
       </c>
       <c r="B44" s="6">
-        <f t="shared" si="3"/>
-        <v>225</v>
+        <f t="shared" si="31"/>
+        <v>224</v>
       </c>
       <c r="C44" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>Phil</v>
       </c>
       <c r="D44" t="str" cm="1">
         <f t="array" aca="1" ref="D44" ca="1">IF(_xlfn.XLOOKUP($B44,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B44,wordle_ids,wordles))</f>
-        <v>WRUNG</v>
+        <v>COULD</v>
       </c>
       <c r="E44" s="10">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
-        <f t="shared" si="4"/>
-        <v>44226</v>
+        <f t="shared" ref="A45:B45" si="32">A38+1</f>
+        <v>44225</v>
       </c>
       <c r="B45" s="6">
-        <f t="shared" si="3"/>
-        <v>225</v>
+        <f t="shared" si="32"/>
+        <v>224</v>
       </c>
       <c r="C45" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>Erik</v>
       </c>
       <c r="D45" t="str" cm="1">
         <f t="array" aca="1" ref="D45" ca="1">IF(_xlfn.XLOOKUP($B45,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B45,wordle_ids,wordles))</f>
-        <v>WRUNG</v>
+        <v>COULD</v>
       </c>
       <c r="E45" s="10">
         <v>4</v>
@@ -1450,62 +1443,62 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
-        <f t="shared" si="4"/>
-        <v>44226</v>
+        <f t="shared" ref="A46:B46" si="33">A39+1</f>
+        <v>44225</v>
       </c>
       <c r="B46" s="6">
-        <f t="shared" si="3"/>
-        <v>225</v>
+        <f t="shared" si="33"/>
+        <v>224</v>
       </c>
       <c r="C46" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>RoBert</v>
       </c>
       <c r="D46" t="str" cm="1">
         <f t="array" aca="1" ref="D46" ca="1">IF(_xlfn.XLOOKUP($B46,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B46,wordle_ids,wordles))</f>
-        <v>WRUNG</v>
+        <v>COULD</v>
       </c>
       <c r="E46" s="10">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
-        <f t="shared" si="4"/>
-        <v>44226</v>
+        <f t="shared" ref="A47:B47" si="34">A40+1</f>
+        <v>44225</v>
       </c>
       <c r="B47" s="6">
-        <f t="shared" si="3"/>
-        <v>225</v>
+        <f t="shared" si="34"/>
+        <v>224</v>
       </c>
       <c r="C47" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>Andrew</v>
       </c>
       <c r="D47" t="str" cm="1">
         <f t="array" aca="1" ref="D47" ca="1">IF(_xlfn.XLOOKUP($B47,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B47,wordle_ids,wordles))</f>
-        <v>WRUNG</v>
+        <v>COULD</v>
       </c>
       <c r="E47" s="10">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
-        <f t="shared" si="4"/>
-        <v>44226</v>
+        <f t="shared" ref="A48:B48" si="35">A41+1</f>
+        <v>44225</v>
       </c>
       <c r="B48" s="6">
-        <f t="shared" si="3"/>
-        <v>225</v>
+        <f t="shared" si="35"/>
+        <v>224</v>
       </c>
       <c r="C48" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>Yoyo</v>
       </c>
       <c r="D48" t="str" cm="1">
         <f t="array" aca="1" ref="D48" ca="1">IF(_xlfn.XLOOKUP($B48,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B48,wordle_ids,wordles))</f>
-        <v>WRUNG</v>
+        <v>COULD</v>
       </c>
       <c r="E48" s="10">
         <v>4</v>
@@ -1513,123 +1506,123 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
-        <f t="shared" si="4"/>
-        <v>44226</v>
+        <f t="shared" ref="A49:B49" si="36">A42+1</f>
+        <v>44225</v>
       </c>
       <c r="B49" s="6">
-        <f t="shared" si="3"/>
-        <v>225</v>
+        <f t="shared" si="36"/>
+        <v>224</v>
       </c>
       <c r="C49" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>Henry</v>
       </c>
       <c r="D49" t="str" cm="1">
         <f t="array" aca="1" ref="D49" ca="1">IF(_xlfn.XLOOKUP($B49,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B49,wordle_ids,wordles))</f>
-        <v>WRUNG</v>
+        <v>COULD</v>
       </c>
       <c r="E49" s="10"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
-        <f t="shared" si="4"/>
-        <v>44227</v>
+        <f t="shared" ref="A50:B50" si="37">A43+1</f>
+        <v>44225</v>
       </c>
       <c r="B50" s="6">
-        <f t="shared" si="3"/>
-        <v>226</v>
+        <f t="shared" si="37"/>
+        <v>224</v>
       </c>
       <c r="C50" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Phil</v>
+        <f t="shared" si="3"/>
+        <v>Aimee</v>
       </c>
       <c r="D50" t="str" cm="1">
         <f t="array" aca="1" ref="D50" ca="1">IF(_xlfn.XLOOKUP($B50,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B50,wordle_ids,wordles))</f>
-        <v>LIGHT</v>
+        <v>COULD</v>
       </c>
       <c r="E50" s="10">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
-        <f t="shared" si="4"/>
-        <v>44227</v>
+        <f t="shared" ref="A51:B51" si="38">A44+1</f>
+        <v>44226</v>
       </c>
       <c r="B51" s="6">
-        <f t="shared" si="3"/>
-        <v>226</v>
+        <f t="shared" si="38"/>
+        <v>225</v>
       </c>
       <c r="C51" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Erik</v>
+        <f t="shared" si="3"/>
+        <v>Phil</v>
       </c>
       <c r="D51" t="str" cm="1">
         <f t="array" aca="1" ref="D51" ca="1">IF(_xlfn.XLOOKUP($B51,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B51,wordle_ids,wordles))</f>
-        <v>LIGHT</v>
+        <v>WRUNG</v>
       </c>
       <c r="E51" s="10">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
-        <f t="shared" si="4"/>
-        <v>44227</v>
+        <f t="shared" ref="A52:B52" si="39">A45+1</f>
+        <v>44226</v>
       </c>
       <c r="B52" s="6">
-        <f t="shared" si="3"/>
-        <v>226</v>
+        <f t="shared" si="39"/>
+        <v>225</v>
       </c>
       <c r="C52" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>RoBert</v>
+        <f t="shared" si="3"/>
+        <v>Erik</v>
       </c>
       <c r="D52" t="str" cm="1">
         <f t="array" aca="1" ref="D52" ca="1">IF(_xlfn.XLOOKUP($B52,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B52,wordle_ids,wordles))</f>
-        <v>LIGHT</v>
+        <v>WRUNG</v>
       </c>
       <c r="E52" s="10">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
-        <f t="shared" si="4"/>
-        <v>44227</v>
+        <f t="shared" ref="A53:B53" si="40">A46+1</f>
+        <v>44226</v>
       </c>
       <c r="B53" s="6">
-        <f t="shared" si="3"/>
-        <v>226</v>
+        <f t="shared" si="40"/>
+        <v>225</v>
       </c>
       <c r="C53" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Andrew</v>
+        <f t="shared" si="3"/>
+        <v>RoBert</v>
       </c>
       <c r="D53" t="str" cm="1">
         <f t="array" aca="1" ref="D53" ca="1">IF(_xlfn.XLOOKUP($B53,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B53,wordle_ids,wordles))</f>
-        <v>LIGHT</v>
+        <v>WRUNG</v>
       </c>
       <c r="E53" s="10">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
-        <f t="shared" si="4"/>
-        <v>44227</v>
+        <f t="shared" ref="A54:B54" si="41">A47+1</f>
+        <v>44226</v>
       </c>
       <c r="B54" s="6">
-        <f t="shared" si="3"/>
-        <v>226</v>
+        <f t="shared" si="41"/>
+        <v>225</v>
       </c>
       <c r="C54" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Yoyo</v>
+        <f t="shared" si="3"/>
+        <v>Andrew</v>
       </c>
       <c r="D54" t="str" cm="1">
         <f t="array" aca="1" ref="D54" ca="1">IF(_xlfn.XLOOKUP($B54,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B54,wordle_ids,wordles))</f>
-        <v>LIGHT</v>
+        <v>WRUNG</v>
       </c>
       <c r="E54" s="10">
         <v>4</v>
@@ -1637,104 +1630,102 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
-        <f>A49+1</f>
-        <v>44227</v>
+        <f t="shared" ref="A55:B55" si="42">A48+1</f>
+        <v>44226</v>
       </c>
       <c r="B55" s="6">
-        <f t="shared" si="3"/>
-        <v>226</v>
+        <f t="shared" si="42"/>
+        <v>225</v>
       </c>
       <c r="C55" s="2" t="str">
-        <f>C49</f>
-        <v>Henry</v>
+        <f t="shared" si="3"/>
+        <v>Yoyo</v>
       </c>
       <c r="D55" t="str" cm="1">
         <f t="array" aca="1" ref="D55" ca="1">IF(_xlfn.XLOOKUP($B55,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B55,wordle_ids,wordles))</f>
-        <v>LIGHT</v>
+        <v>WRUNG</v>
       </c>
       <c r="E55" s="10">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
-        <f t="shared" si="4"/>
-        <v>44228</v>
+        <f t="shared" ref="A56:B56" si="43">A49+1</f>
+        <v>44226</v>
       </c>
       <c r="B56" s="6">
-        <f t="shared" si="3"/>
-        <v>227</v>
+        <f t="shared" si="43"/>
+        <v>225</v>
       </c>
       <c r="C56" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Phil</v>
+        <f t="shared" si="3"/>
+        <v>Henry</v>
       </c>
       <c r="D56" t="str" cm="1">
         <f t="array" aca="1" ref="D56" ca="1">IF(_xlfn.XLOOKUP($B56,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B56,wordle_ids,wordles))</f>
-        <v>THOSE</v>
-      </c>
-      <c r="E56" s="10">
-        <v>2</v>
-      </c>
+        <v>WRUNG</v>
+      </c>
+      <c r="E56" s="10"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
-        <f t="shared" si="4"/>
-        <v>44228</v>
+        <f t="shared" ref="A57:B57" si="44">A50+1</f>
+        <v>44226</v>
       </c>
       <c r="B57" s="6">
-        <f t="shared" si="3"/>
-        <v>227</v>
+        <f t="shared" si="44"/>
+        <v>225</v>
       </c>
       <c r="C57" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Erik</v>
+        <f t="shared" si="3"/>
+        <v>Aimee</v>
       </c>
       <c r="D57" t="str" cm="1">
         <f t="array" aca="1" ref="D57" ca="1">IF(_xlfn.XLOOKUP($B57,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B57,wordle_ids,wordles))</f>
-        <v>THOSE</v>
+        <v>WRUNG</v>
       </c>
       <c r="E57" s="10">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
-        <f t="shared" si="4"/>
-        <v>44228</v>
+        <f t="shared" ref="A58:B58" si="45">A51+1</f>
+        <v>44227</v>
       </c>
       <c r="B58" s="6">
-        <f t="shared" si="3"/>
-        <v>227</v>
+        <f t="shared" si="45"/>
+        <v>226</v>
       </c>
       <c r="C58" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>RoBert</v>
+        <f t="shared" si="3"/>
+        <v>Phil</v>
       </c>
       <c r="D58" t="str" cm="1">
         <f t="array" aca="1" ref="D58" ca="1">IF(_xlfn.XLOOKUP($B58,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B58,wordle_ids,wordles))</f>
-        <v>THOSE</v>
+        <v>LIGHT</v>
       </c>
       <c r="E58" s="10">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
-        <f t="shared" si="4"/>
-        <v>44228</v>
+        <f t="shared" ref="A59:B59" si="46">A52+1</f>
+        <v>44227</v>
       </c>
       <c r="B59" s="6">
-        <f t="shared" si="3"/>
-        <v>227</v>
+        <f t="shared" si="46"/>
+        <v>226</v>
       </c>
       <c r="C59" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Andrew</v>
+        <f t="shared" si="3"/>
+        <v>Erik</v>
       </c>
       <c r="D59" t="str" cm="1">
         <f t="array" aca="1" ref="D59" ca="1">IF(_xlfn.XLOOKUP($B59,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B59,wordle_ids,wordles))</f>
-        <v>THOSE</v>
+        <v>LIGHT</v>
       </c>
       <c r="E59" s="10">
         <v>4</v>
@@ -1742,20 +1733,20 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
-        <f t="shared" si="4"/>
-        <v>44228</v>
+        <f t="shared" ref="A60:B60" si="47">A53+1</f>
+        <v>44227</v>
       </c>
       <c r="B60" s="6">
-        <f t="shared" si="3"/>
-        <v>227</v>
+        <f t="shared" si="47"/>
+        <v>226</v>
       </c>
       <c r="C60" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Yoyo</v>
+        <f t="shared" si="3"/>
+        <v>RoBert</v>
       </c>
       <c r="D60" t="str" cm="1">
         <f t="array" aca="1" ref="D60" ca="1">IF(_xlfn.XLOOKUP($B60,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B60,wordle_ids,wordles))</f>
-        <v>THOSE</v>
+        <v>LIGHT</v>
       </c>
       <c r="E60" s="10">
         <v>3</v>
@@ -1763,83 +1754,83 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
-        <f t="shared" si="4"/>
-        <v>44228</v>
+        <f t="shared" ref="A61:B61" si="48">A54+1</f>
+        <v>44227</v>
       </c>
       <c r="B61" s="6">
-        <f t="shared" si="3"/>
-        <v>227</v>
+        <f t="shared" si="48"/>
+        <v>226</v>
       </c>
       <c r="C61" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Henry</v>
+        <f t="shared" si="3"/>
+        <v>Andrew</v>
       </c>
       <c r="D61" t="str" cm="1">
         <f t="array" aca="1" ref="D61" ca="1">IF(_xlfn.XLOOKUP($B61,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B61,wordle_ids,wordles))</f>
-        <v>THOSE</v>
+        <v>LIGHT</v>
       </c>
       <c r="E61" s="10">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
-        <f t="shared" si="4"/>
-        <v>44229</v>
+        <f t="shared" ref="A62:B62" si="49">A55+1</f>
+        <v>44227</v>
       </c>
       <c r="B62" s="6">
-        <f t="shared" si="3"/>
-        <v>228</v>
+        <f t="shared" si="49"/>
+        <v>226</v>
       </c>
       <c r="C62" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Phil</v>
+        <f t="shared" si="3"/>
+        <v>Yoyo</v>
       </c>
       <c r="D62" t="str" cm="1">
         <f t="array" aca="1" ref="D62" ca="1">IF(_xlfn.XLOOKUP($B62,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B62,wordle_ids,wordles))</f>
-        <v>MOIST</v>
+        <v>LIGHT</v>
       </c>
       <c r="E62" s="10">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
-        <f t="shared" si="4"/>
-        <v>44229</v>
+        <f t="shared" ref="A63:B63" si="50">A56+1</f>
+        <v>44227</v>
       </c>
       <c r="B63" s="6">
-        <f t="shared" si="3"/>
-        <v>228</v>
+        <f t="shared" si="50"/>
+        <v>226</v>
       </c>
       <c r="C63" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Erik</v>
+        <f t="shared" si="3"/>
+        <v>Henry</v>
       </c>
       <c r="D63" t="str" cm="1">
         <f t="array" aca="1" ref="D63" ca="1">IF(_xlfn.XLOOKUP($B63,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B63,wordle_ids,wordles))</f>
-        <v>MOIST</v>
+        <v>LIGHT</v>
       </c>
       <c r="E63" s="10">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
-        <f t="shared" si="4"/>
-        <v>44229</v>
+        <f t="shared" ref="A64:B64" si="51">A57+1</f>
+        <v>44227</v>
       </c>
       <c r="B64" s="6">
-        <f t="shared" si="3"/>
-        <v>228</v>
+        <f t="shared" si="51"/>
+        <v>226</v>
       </c>
       <c r="C64" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>RoBert</v>
+        <f t="shared" si="3"/>
+        <v>Aimee</v>
       </c>
       <c r="D64" t="str" cm="1">
         <f t="array" aca="1" ref="D64" ca="1">IF(_xlfn.XLOOKUP($B64,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B64,wordle_ids,wordles))</f>
-        <v>MOIST</v>
+        <v>LIGHT</v>
       </c>
       <c r="E64" s="10">
         <v>3</v>
@@ -1847,377 +1838,375 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
-        <f t="shared" si="4"/>
-        <v>44229</v>
+        <f t="shared" ref="A65:B65" si="52">A58+1</f>
+        <v>44228</v>
       </c>
       <c r="B65" s="6">
-        <f t="shared" si="3"/>
-        <v>228</v>
+        <f t="shared" si="52"/>
+        <v>227</v>
       </c>
       <c r="C65" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Andrew</v>
+        <f t="shared" si="3"/>
+        <v>Phil</v>
       </c>
       <c r="D65" t="str" cm="1">
         <f t="array" aca="1" ref="D65" ca="1">IF(_xlfn.XLOOKUP($B65,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B65,wordle_ids,wordles))</f>
-        <v>MOIST</v>
+        <v>THOSE</v>
       </c>
       <c r="E65" s="10">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
-        <f t="shared" si="4"/>
-        <v>44229</v>
+        <f t="shared" ref="A66:B66" si="53">A59+1</f>
+        <v>44228</v>
       </c>
       <c r="B66" s="6">
-        <f t="shared" si="3"/>
-        <v>228</v>
+        <f t="shared" si="53"/>
+        <v>227</v>
       </c>
       <c r="C66" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Yoyo</v>
+        <f t="shared" si="3"/>
+        <v>Erik</v>
       </c>
       <c r="D66" t="str" cm="1">
         <f t="array" aca="1" ref="D66" ca="1">IF(_xlfn.XLOOKUP($B66,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B66,wordle_ids,wordles))</f>
-        <v>MOIST</v>
+        <v>THOSE</v>
       </c>
       <c r="E66" s="10">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
-        <f t="shared" si="4"/>
-        <v>44229</v>
+        <f t="shared" ref="A67:B67" si="54">A60+1</f>
+        <v>44228</v>
       </c>
       <c r="B67" s="6">
-        <f t="shared" si="3"/>
-        <v>228</v>
+        <f t="shared" si="54"/>
+        <v>227</v>
       </c>
       <c r="C67" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Henry</v>
+        <f t="shared" si="3"/>
+        <v>RoBert</v>
       </c>
       <c r="D67" t="str" cm="1">
         <f t="array" aca="1" ref="D67" ca="1">IF(_xlfn.XLOOKUP($B67,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B67,wordle_ids,wordles))</f>
-        <v>MOIST</v>
+        <v>THOSE</v>
       </c>
       <c r="E67" s="10">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
-        <f t="shared" si="4"/>
-        <v>44230</v>
+        <f t="shared" ref="A68:B68" si="55">A61+1</f>
+        <v>44228</v>
       </c>
       <c r="B68" s="6">
-        <f t="shared" si="3"/>
-        <v>229</v>
+        <f t="shared" si="55"/>
+        <v>227</v>
       </c>
       <c r="C68" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Phil</v>
+        <f t="shared" si="3"/>
+        <v>Andrew</v>
       </c>
       <c r="D68" t="str" cm="1">
         <f t="array" aca="1" ref="D68" ca="1">IF(_xlfn.XLOOKUP($B68,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B68,wordle_ids,wordles))</f>
-        <v>SHARD</v>
+        <v>THOSE</v>
       </c>
       <c r="E68" s="10">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
-        <f t="shared" si="4"/>
-        <v>44230</v>
+        <f t="shared" ref="A69:B69" si="56">A62+1</f>
+        <v>44228</v>
       </c>
       <c r="B69" s="6">
-        <f t="shared" si="3"/>
-        <v>229</v>
+        <f t="shared" si="56"/>
+        <v>227</v>
       </c>
       <c r="C69" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Erik</v>
+        <f t="shared" si="3"/>
+        <v>Yoyo</v>
       </c>
       <c r="D69" t="str" cm="1">
         <f t="array" aca="1" ref="D69" ca="1">IF(_xlfn.XLOOKUP($B69,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B69,wordle_ids,wordles))</f>
-        <v>SHARD</v>
+        <v>THOSE</v>
       </c>
       <c r="E69" s="10">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
-        <f t="shared" si="4"/>
-        <v>44230</v>
+        <f t="shared" ref="A70:B70" si="57">A63+1</f>
+        <v>44228</v>
       </c>
       <c r="B70" s="6">
-        <f t="shared" si="3"/>
-        <v>229</v>
+        <f t="shared" si="57"/>
+        <v>227</v>
       </c>
       <c r="C70" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>RoBert</v>
+        <f t="shared" si="3"/>
+        <v>Henry</v>
       </c>
       <c r="D70" t="str" cm="1">
         <f t="array" aca="1" ref="D70" ca="1">IF(_xlfn.XLOOKUP($B70,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B70,wordle_ids,wordles))</f>
-        <v>SHARD</v>
+        <v>THOSE</v>
       </c>
       <c r="E70" s="10">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
-        <f t="shared" si="4"/>
-        <v>44230</v>
+        <f t="shared" ref="A71:B71" si="58">A64+1</f>
+        <v>44228</v>
       </c>
       <c r="B71" s="6">
-        <f t="shared" si="3"/>
-        <v>229</v>
+        <f t="shared" si="58"/>
+        <v>227</v>
       </c>
       <c r="C71" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Andrew</v>
+        <f t="shared" si="3"/>
+        <v>Aimee</v>
       </c>
       <c r="D71" t="str" cm="1">
         <f t="array" aca="1" ref="D71" ca="1">IF(_xlfn.XLOOKUP($B71,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B71,wordle_ids,wordles))</f>
-        <v>SHARD</v>
-      </c>
-      <c r="E71" s="10">
-        <v>4</v>
-      </c>
+        <v>THOSE</v>
+      </c>
+      <c r="E71" s="10"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
-        <f t="shared" si="4"/>
-        <v>44230</v>
+        <f t="shared" ref="A72:B72" si="59">A65+1</f>
+        <v>44229</v>
       </c>
       <c r="B72" s="6">
-        <f t="shared" si="3"/>
-        <v>229</v>
+        <f t="shared" si="59"/>
+        <v>228</v>
       </c>
       <c r="C72" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Yoyo</v>
+        <f t="shared" si="3"/>
+        <v>Phil</v>
       </c>
       <c r="D72" t="str" cm="1">
         <f t="array" aca="1" ref="D72" ca="1">IF(_xlfn.XLOOKUP($B72,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B72,wordle_ids,wordles))</f>
-        <v>SHARD</v>
+        <v>MOIST</v>
       </c>
       <c r="E72" s="10">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
-        <f t="shared" si="4"/>
-        <v>44230</v>
+        <f t="shared" ref="A73:B73" si="60">A66+1</f>
+        <v>44229</v>
       </c>
       <c r="B73" s="6">
-        <f t="shared" si="3"/>
-        <v>229</v>
+        <f t="shared" si="60"/>
+        <v>228</v>
       </c>
       <c r="C73" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Henry</v>
+        <f t="shared" si="3"/>
+        <v>Erik</v>
       </c>
       <c r="D73" t="str" cm="1">
         <f t="array" aca="1" ref="D73" ca="1">IF(_xlfn.XLOOKUP($B73,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B73,wordle_ids,wordles))</f>
-        <v>SHARD</v>
+        <v>MOIST</v>
       </c>
       <c r="E73" s="10">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
-        <f t="shared" si="4"/>
-        <v>44231</v>
+        <f t="shared" ref="A74:B74" si="61">A67+1</f>
+        <v>44229</v>
       </c>
       <c r="B74" s="6">
-        <f t="shared" si="3"/>
-        <v>230</v>
+        <f t="shared" si="61"/>
+        <v>228</v>
       </c>
       <c r="C74" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Phil</v>
+        <f t="shared" si="3"/>
+        <v>RoBert</v>
       </c>
       <c r="D74" t="str" cm="1">
         <f t="array" aca="1" ref="D74" ca="1">IF(_xlfn.XLOOKUP($B74,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B74,wordle_ids,wordles))</f>
-        <v>PLEAT</v>
+        <v>MOIST</v>
       </c>
       <c r="E74" s="10">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
-        <f t="shared" si="4"/>
-        <v>44231</v>
+        <f t="shared" ref="A75:B75" si="62">A68+1</f>
+        <v>44229</v>
       </c>
       <c r="B75" s="6">
-        <f t="shared" si="3"/>
-        <v>230</v>
+        <f t="shared" si="62"/>
+        <v>228</v>
       </c>
       <c r="C75" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Erik</v>
+        <f t="shared" si="3"/>
+        <v>Andrew</v>
       </c>
       <c r="D75" t="str" cm="1">
         <f t="array" aca="1" ref="D75" ca="1">IF(_xlfn.XLOOKUP($B75,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B75,wordle_ids,wordles))</f>
-        <v>PLEAT</v>
+        <v>MOIST</v>
       </c>
       <c r="E75" s="10">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
-        <f t="shared" si="4"/>
-        <v>44231</v>
+        <f t="shared" ref="A76:B76" si="63">A69+1</f>
+        <v>44229</v>
       </c>
       <c r="B76" s="6">
-        <f t="shared" si="3"/>
-        <v>230</v>
+        <f t="shared" si="63"/>
+        <v>228</v>
       </c>
       <c r="C76" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>RoBert</v>
+        <f t="shared" si="3"/>
+        <v>Yoyo</v>
       </c>
       <c r="D76" t="str" cm="1">
         <f t="array" aca="1" ref="D76" ca="1">IF(_xlfn.XLOOKUP($B76,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B76,wordle_ids,wordles))</f>
-        <v>PLEAT</v>
+        <v>MOIST</v>
       </c>
       <c r="E76" s="10">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
-        <f t="shared" si="4"/>
-        <v>44231</v>
+        <f t="shared" ref="A77:B77" si="64">A70+1</f>
+        <v>44229</v>
       </c>
       <c r="B77" s="6">
-        <f t="shared" si="3"/>
-        <v>230</v>
+        <f t="shared" si="64"/>
+        <v>228</v>
       </c>
       <c r="C77" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Andrew</v>
+        <f t="shared" si="3"/>
+        <v>Henry</v>
       </c>
       <c r="D77" t="str" cm="1">
         <f t="array" aca="1" ref="D77" ca="1">IF(_xlfn.XLOOKUP($B77,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B77,wordle_ids,wordles))</f>
-        <v>PLEAT</v>
+        <v>MOIST</v>
       </c>
       <c r="E77" s="10">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
-        <f t="shared" si="4"/>
-        <v>44231</v>
+        <f t="shared" ref="A78:B78" si="65">A71+1</f>
+        <v>44229</v>
       </c>
       <c r="B78" s="6">
-        <f t="shared" si="3"/>
-        <v>230</v>
+        <f t="shared" si="65"/>
+        <v>228</v>
       </c>
       <c r="C78" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Yoyo</v>
+        <f t="shared" si="3"/>
+        <v>Aimee</v>
       </c>
       <c r="D78" t="str" cm="1">
         <f t="array" aca="1" ref="D78" ca="1">IF(_xlfn.XLOOKUP($B78,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B78,wordle_ids,wordles))</f>
-        <v>PLEAT</v>
+        <v>MOIST</v>
       </c>
       <c r="E78" s="10">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
-        <f t="shared" si="4"/>
-        <v>44231</v>
+        <f t="shared" ref="A79:B79" si="66">A72+1</f>
+        <v>44230</v>
       </c>
       <c r="B79" s="6">
-        <f t="shared" si="3"/>
-        <v>230</v>
+        <f t="shared" si="66"/>
+        <v>229</v>
       </c>
       <c r="C79" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Henry</v>
+        <f t="shared" si="3"/>
+        <v>Phil</v>
       </c>
       <c r="D79" t="str" cm="1">
         <f t="array" aca="1" ref="D79" ca="1">IF(_xlfn.XLOOKUP($B79,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B79,wordle_ids,wordles))</f>
-        <v>PLEAT</v>
+        <v>SHARD</v>
       </c>
       <c r="E79" s="10">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
-        <f t="shared" si="4"/>
-        <v>44232</v>
+        <f t="shared" ref="A80:B80" si="67">A73+1</f>
+        <v>44230</v>
       </c>
       <c r="B80" s="6">
-        <f t="shared" si="3"/>
-        <v>231</v>
+        <f t="shared" si="67"/>
+        <v>229</v>
       </c>
       <c r="C80" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Phil</v>
+        <f t="shared" si="3"/>
+        <v>Erik</v>
       </c>
       <c r="D80" t="str" cm="1">
         <f t="array" aca="1" ref="D80" ca="1">IF(_xlfn.XLOOKUP($B80,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B80,wordle_ids,wordles))</f>
-        <v>ALOFT</v>
-      </c>
-      <c r="E80" s="10" t="s">
-        <v>18</v>
+        <v>SHARD</v>
+      </c>
+      <c r="E80" s="10">
+        <v>5</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
-        <f t="shared" si="4"/>
-        <v>44232</v>
+        <f t="shared" ref="A81:B81" si="68">A74+1</f>
+        <v>44230</v>
       </c>
       <c r="B81" s="6">
-        <f t="shared" si="3"/>
-        <v>231</v>
+        <f t="shared" si="68"/>
+        <v>229</v>
       </c>
       <c r="C81" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Erik</v>
+        <f t="shared" si="3"/>
+        <v>RoBert</v>
       </c>
       <c r="D81" t="str" cm="1">
         <f t="array" aca="1" ref="D81" ca="1">IF(_xlfn.XLOOKUP($B81,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B81,wordle_ids,wordles))</f>
-        <v>ALOFT</v>
+        <v>SHARD</v>
       </c>
       <c r="E81" s="10">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
-        <f t="shared" si="4"/>
-        <v>44232</v>
+        <f t="shared" ref="A82:B82" si="69">A75+1</f>
+        <v>44230</v>
       </c>
       <c r="B82" s="6">
-        <f t="shared" si="3"/>
-        <v>231</v>
+        <f t="shared" si="69"/>
+        <v>229</v>
       </c>
       <c r="C82" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>RoBert</v>
+        <f t="shared" si="3"/>
+        <v>Andrew</v>
       </c>
       <c r="D82" t="str" cm="1">
         <f t="array" aca="1" ref="D82" ca="1">IF(_xlfn.XLOOKUP($B82,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B82,wordle_ids,wordles))</f>
-        <v>ALOFT</v>
+        <v>SHARD</v>
       </c>
       <c r="E82" s="10">
         <v>4</v>
@@ -2225,20 +2214,20 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
-        <f t="shared" si="4"/>
-        <v>44232</v>
+        <f t="shared" ref="A83:B83" si="70">A76+1</f>
+        <v>44230</v>
       </c>
       <c r="B83" s="6">
-        <f t="shared" si="3"/>
-        <v>231</v>
+        <f t="shared" si="70"/>
+        <v>229</v>
       </c>
       <c r="C83" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Andrew</v>
+        <f t="shared" si="3"/>
+        <v>Yoyo</v>
       </c>
       <c r="D83" t="str" cm="1">
         <f t="array" aca="1" ref="D83" ca="1">IF(_xlfn.XLOOKUP($B83,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B83,wordle_ids,wordles))</f>
-        <v>ALOFT</v>
+        <v>SHARD</v>
       </c>
       <c r="E83" s="10">
         <v>4</v>
@@ -2246,20 +2235,20 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
-        <f t="shared" si="4"/>
-        <v>44232</v>
+        <f t="shared" ref="A84:B84" si="71">A77+1</f>
+        <v>44230</v>
       </c>
       <c r="B84" s="6">
-        <f t="shared" si="3"/>
-        <v>231</v>
+        <f t="shared" si="71"/>
+        <v>229</v>
       </c>
       <c r="C84" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Yoyo</v>
+        <f t="shared" si="3"/>
+        <v>Henry</v>
       </c>
       <c r="D84" t="str" cm="1">
         <f t="array" aca="1" ref="D84" ca="1">IF(_xlfn.XLOOKUP($B84,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B84,wordle_ids,wordles))</f>
-        <v>ALOFT</v>
+        <v>SHARD</v>
       </c>
       <c r="E84" s="10">
         <v>4</v>
@@ -2267,20 +2256,20 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
-        <f t="shared" si="4"/>
-        <v>44232</v>
+        <f t="shared" ref="A85:B85" si="72">A78+1</f>
+        <v>44230</v>
       </c>
       <c r="B85" s="6">
-        <f t="shared" si="3"/>
-        <v>231</v>
+        <f t="shared" si="72"/>
+        <v>229</v>
       </c>
       <c r="C85" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Henry</v>
+        <f t="shared" si="3"/>
+        <v>Aimee</v>
       </c>
       <c r="D85" t="str" cm="1">
         <f t="array" aca="1" ref="D85" ca="1">IF(_xlfn.XLOOKUP($B85,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B85,wordle_ids,wordles))</f>
-        <v>ALOFT</v>
+        <v>SHARD</v>
       </c>
       <c r="E85" s="10">
         <v>4</v>
@@ -2288,41 +2277,41 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
-        <f t="shared" si="4"/>
-        <v>44233</v>
+        <f t="shared" ref="A86:B86" si="73">A79+1</f>
+        <v>44231</v>
       </c>
       <c r="B86" s="6">
-        <f t="shared" si="3"/>
-        <v>232</v>
+        <f t="shared" si="73"/>
+        <v>230</v>
       </c>
       <c r="C86" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>Phil</v>
       </c>
       <c r="D86" t="str" cm="1">
         <f t="array" aca="1" ref="D86" ca="1">IF(_xlfn.XLOOKUP($B86,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B86,wordle_ids,wordles))</f>
-        <v>SKILL</v>
+        <v>PLEAT</v>
       </c>
       <c r="E86" s="10">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
-        <f t="shared" si="4"/>
-        <v>44233</v>
+        <f t="shared" ref="A87:B87" si="74">A80+1</f>
+        <v>44231</v>
       </c>
       <c r="B87" s="6">
-        <f t="shared" si="3"/>
-        <v>232</v>
+        <f t="shared" si="74"/>
+        <v>230</v>
       </c>
       <c r="C87" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="C87" si="75">C80</f>
         <v>Erik</v>
       </c>
       <c r="D87" t="str" cm="1">
         <f t="array" aca="1" ref="D87" ca="1">IF(_xlfn.XLOOKUP($B87,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B87,wordle_ids,wordles))</f>
-        <v>SKILL</v>
+        <v>PLEAT</v>
       </c>
       <c r="E87" s="10">
         <v>5</v>
@@ -2330,41 +2319,41 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
-        <f t="shared" si="4"/>
-        <v>44233</v>
+        <f t="shared" ref="A88:B88" si="76">A81+1</f>
+        <v>44231</v>
       </c>
       <c r="B88" s="6">
-        <f t="shared" si="3"/>
-        <v>232</v>
+        <f t="shared" si="76"/>
+        <v>230</v>
       </c>
       <c r="C88" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>RoBert</v>
       </c>
       <c r="D88" t="str" cm="1">
         <f t="array" aca="1" ref="D88" ca="1">IF(_xlfn.XLOOKUP($B88,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B88,wordle_ids,wordles))</f>
-        <v>SKILL</v>
+        <v>PLEAT</v>
       </c>
       <c r="E88" s="10">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
-        <f t="shared" si="4"/>
-        <v>44233</v>
+        <f t="shared" ref="A89:B89" si="77">A82+1</f>
+        <v>44231</v>
       </c>
       <c r="B89" s="6">
-        <f t="shared" si="3"/>
-        <v>232</v>
+        <f t="shared" si="77"/>
+        <v>230</v>
       </c>
       <c r="C89" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>Andrew</v>
       </c>
       <c r="D89" t="str" cm="1">
         <f t="array" aca="1" ref="D89" ca="1">IF(_xlfn.XLOOKUP($B89,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B89,wordle_ids,wordles))</f>
-        <v>SKILL</v>
+        <v>PLEAT</v>
       </c>
       <c r="E89" s="10">
         <v>5</v>
@@ -2372,164 +2361,560 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
-        <f t="shared" si="4"/>
-        <v>44233</v>
+        <f t="shared" ref="A90:B90" si="78">A83+1</f>
+        <v>44231</v>
       </c>
       <c r="B90" s="6">
-        <f t="shared" si="3"/>
-        <v>232</v>
+        <f t="shared" si="78"/>
+        <v>230</v>
       </c>
       <c r="C90" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>Yoyo</v>
       </c>
       <c r="D90" t="str" cm="1">
         <f t="array" aca="1" ref="D90" ca="1">IF(_xlfn.XLOOKUP($B90,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B90,wordle_ids,wordles))</f>
-        <v>SKILL</v>
+        <v>PLEAT</v>
       </c>
       <c r="E90" s="10">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
-        <f t="shared" si="4"/>
-        <v>44233</v>
+        <f t="shared" ref="A91:B91" si="79">A84+1</f>
+        <v>44231</v>
       </c>
       <c r="B91" s="6">
-        <f t="shared" si="3"/>
-        <v>232</v>
+        <f t="shared" si="79"/>
+        <v>230</v>
       </c>
       <c r="C91" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>Henry</v>
       </c>
       <c r="D91" t="str" cm="1">
         <f t="array" aca="1" ref="D91" ca="1">IF(_xlfn.XLOOKUP($B91,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B91,wordle_ids,wordles))</f>
+        <v>PLEAT</v>
+      </c>
+      <c r="E91" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="2">
+        <f t="shared" ref="A92:B92" si="80">A85+1</f>
+        <v>44231</v>
+      </c>
+      <c r="B92" s="6">
+        <f t="shared" si="80"/>
+        <v>230</v>
+      </c>
+      <c r="C92" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>Aimee</v>
+      </c>
+      <c r="D92" t="str" cm="1">
+        <f t="array" aca="1" ref="D92" ca="1">IF(_xlfn.XLOOKUP($B92,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B92,wordle_ids,wordles))</f>
+        <v>PLEAT</v>
+      </c>
+      <c r="E92" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="2">
+        <f t="shared" ref="A93:B93" si="81">A86+1</f>
+        <v>44232</v>
+      </c>
+      <c r="B93" s="6">
+        <f t="shared" si="81"/>
+        <v>231</v>
+      </c>
+      <c r="C93" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>Phil</v>
+      </c>
+      <c r="D93" t="str" cm="1">
+        <f t="array" aca="1" ref="D93" ca="1">IF(_xlfn.XLOOKUP($B93,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B93,wordle_ids,wordles))</f>
+        <v>ALOFT</v>
+      </c>
+      <c r="E93" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="2">
+        <f t="shared" ref="A94:B94" si="82">A87+1</f>
+        <v>44232</v>
+      </c>
+      <c r="B94" s="6">
+        <f t="shared" si="82"/>
+        <v>231</v>
+      </c>
+      <c r="C94" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>Erik</v>
+      </c>
+      <c r="D94" t="str" cm="1">
+        <f t="array" aca="1" ref="D94" ca="1">IF(_xlfn.XLOOKUP($B94,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B94,wordle_ids,wordles))</f>
+        <v>ALOFT</v>
+      </c>
+      <c r="E94" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="2">
+        <f t="shared" ref="A95:B95" si="83">A88+1</f>
+        <v>44232</v>
+      </c>
+      <c r="B95" s="6">
+        <f t="shared" si="83"/>
+        <v>231</v>
+      </c>
+      <c r="C95" s="2" t="str">
+        <f t="shared" ref="C95" si="84">C88</f>
+        <v>RoBert</v>
+      </c>
+      <c r="D95" t="str" cm="1">
+        <f t="array" aca="1" ref="D95" ca="1">IF(_xlfn.XLOOKUP($B95,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B95,wordle_ids,wordles))</f>
+        <v>ALOFT</v>
+      </c>
+      <c r="E95" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="2">
+        <f t="shared" ref="A96:B96" si="85">A89+1</f>
+        <v>44232</v>
+      </c>
+      <c r="B96" s="6">
+        <f t="shared" si="85"/>
+        <v>231</v>
+      </c>
+      <c r="C96" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>Andrew</v>
+      </c>
+      <c r="D96" t="str" cm="1">
+        <f t="array" aca="1" ref="D96" ca="1">IF(_xlfn.XLOOKUP($B96,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B96,wordle_ids,wordles))</f>
+        <v>ALOFT</v>
+      </c>
+      <c r="E96" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="2">
+        <f t="shared" ref="A97:B97" si="86">A90+1</f>
+        <v>44232</v>
+      </c>
+      <c r="B97" s="6">
+        <f t="shared" si="86"/>
+        <v>231</v>
+      </c>
+      <c r="C97" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>Yoyo</v>
+      </c>
+      <c r="D97" t="str" cm="1">
+        <f t="array" aca="1" ref="D97" ca="1">IF(_xlfn.XLOOKUP($B97,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B97,wordle_ids,wordles))</f>
+        <v>ALOFT</v>
+      </c>
+      <c r="E97" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" s="2">
+        <f t="shared" ref="A98:B98" si="87">A91+1</f>
+        <v>44232</v>
+      </c>
+      <c r="B98" s="6">
+        <f t="shared" si="87"/>
+        <v>231</v>
+      </c>
+      <c r="C98" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>Henry</v>
+      </c>
+      <c r="D98" t="str" cm="1">
+        <f t="array" aca="1" ref="D98" ca="1">IF(_xlfn.XLOOKUP($B98,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B98,wordle_ids,wordles))</f>
+        <v>ALOFT</v>
+      </c>
+      <c r="E98" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="2">
+        <f t="shared" ref="A99:B99" si="88">A92+1</f>
+        <v>44232</v>
+      </c>
+      <c r="B99" s="6">
+        <f t="shared" si="88"/>
+        <v>231</v>
+      </c>
+      <c r="C99" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>Aimee</v>
+      </c>
+      <c r="D99" t="str" cm="1">
+        <f t="array" aca="1" ref="D99" ca="1">IF(_xlfn.XLOOKUP($B99,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B99,wordle_ids,wordles))</f>
+        <v>ALOFT</v>
+      </c>
+      <c r="E99" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" s="2">
+        <f t="shared" ref="A100:B100" si="89">A93+1</f>
+        <v>44233</v>
+      </c>
+      <c r="B100" s="6">
+        <f t="shared" si="89"/>
+        <v>232</v>
+      </c>
+      <c r="C100" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>Phil</v>
+      </c>
+      <c r="D100" t="str" cm="1">
+        <f t="array" aca="1" ref="D100" ca="1">IF(_xlfn.XLOOKUP($B100,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B100,wordle_ids,wordles))</f>
         <v>SKILL</v>
       </c>
-      <c r="E91" s="10">
+      <c r="E100" s="10">
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="2"/>
-      <c r="B92" s="6"/>
-      <c r="C92" s="2"/>
-      <c r="E92" s="10"/>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" s="2"/>
-      <c r="B93" s="6"/>
-      <c r="C93" s="2"/>
-      <c r="E93" s="10"/>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" s="2"/>
-      <c r="B94" s="6"/>
-      <c r="C94" s="2"/>
-      <c r="E94" s="10"/>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E95" s="10"/>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E96" s="10"/>
-    </row>
-    <row r="97" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E97" s="10"/>
-    </row>
-    <row r="98" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E98" s="10"/>
-    </row>
-    <row r="99" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E99" s="10"/>
-    </row>
-    <row r="100" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E100" s="10"/>
-    </row>
-    <row r="101" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E101" s="10"/>
-    </row>
-    <row r="102" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E102" s="10"/>
-    </row>
-    <row r="103" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E103" s="10"/>
-    </row>
-    <row r="104" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E104" s="10"/>
-    </row>
-    <row r="105" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E105" s="10"/>
-    </row>
-    <row r="106" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E106" s="10"/>
-    </row>
-    <row r="107" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E107" s="10"/>
-    </row>
-    <row r="108" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E108" s="10"/>
-    </row>
-    <row r="109" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E109" s="10"/>
-    </row>
-    <row r="110" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E110" s="10"/>
-    </row>
-    <row r="111" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E111" s="10"/>
-    </row>
-    <row r="112" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E112" s="10"/>
-    </row>
-    <row r="113" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E113" s="10"/>
-    </row>
-    <row r="114" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="2">
+        <f t="shared" ref="A101:B101" si="90">A94+1</f>
+        <v>44233</v>
+      </c>
+      <c r="B101" s="6">
+        <f t="shared" si="90"/>
+        <v>232</v>
+      </c>
+      <c r="C101" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>Erik</v>
+      </c>
+      <c r="D101" t="str" cm="1">
+        <f t="array" aca="1" ref="D101" ca="1">IF(_xlfn.XLOOKUP($B101,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B101,wordle_ids,wordles))</f>
+        <v>SKILL</v>
+      </c>
+      <c r="E101" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" s="2">
+        <f t="shared" ref="A102:B102" si="91">A95+1</f>
+        <v>44233</v>
+      </c>
+      <c r="B102" s="6">
+        <f t="shared" si="91"/>
+        <v>232</v>
+      </c>
+      <c r="C102" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>RoBert</v>
+      </c>
+      <c r="D102" t="str" cm="1">
+        <f t="array" aca="1" ref="D102" ca="1">IF(_xlfn.XLOOKUP($B102,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B102,wordle_ids,wordles))</f>
+        <v>SKILL</v>
+      </c>
+      <c r="E102" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" s="2">
+        <f t="shared" ref="A103:B103" si="92">A96+1</f>
+        <v>44233</v>
+      </c>
+      <c r="B103" s="6">
+        <f t="shared" si="92"/>
+        <v>232</v>
+      </c>
+      <c r="C103" s="2" t="str">
+        <f t="shared" ref="C103" si="93">C96</f>
+        <v>Andrew</v>
+      </c>
+      <c r="D103" t="str" cm="1">
+        <f t="array" aca="1" ref="D103" ca="1">IF(_xlfn.XLOOKUP($B103,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B103,wordle_ids,wordles))</f>
+        <v>SKILL</v>
+      </c>
+      <c r="E103" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="2">
+        <f t="shared" ref="A104:B104" si="94">A97+1</f>
+        <v>44233</v>
+      </c>
+      <c r="B104" s="6">
+        <f t="shared" si="94"/>
+        <v>232</v>
+      </c>
+      <c r="C104" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>Yoyo</v>
+      </c>
+      <c r="D104" t="str" cm="1">
+        <f t="array" aca="1" ref="D104" ca="1">IF(_xlfn.XLOOKUP($B104,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B104,wordle_ids,wordles))</f>
+        <v>SKILL</v>
+      </c>
+      <c r="E104" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" s="2">
+        <f t="shared" ref="A105:B105" si="95">A98+1</f>
+        <v>44233</v>
+      </c>
+      <c r="B105" s="6">
+        <f t="shared" si="95"/>
+        <v>232</v>
+      </c>
+      <c r="C105" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>Henry</v>
+      </c>
+      <c r="D105" t="str" cm="1">
+        <f t="array" aca="1" ref="D105" ca="1">IF(_xlfn.XLOOKUP($B105,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B105,wordle_ids,wordles))</f>
+        <v>SKILL</v>
+      </c>
+      <c r="E105" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" s="2">
+        <f t="shared" ref="A106:B106" si="96">A99+1</f>
+        <v>44233</v>
+      </c>
+      <c r="B106" s="6">
+        <f t="shared" si="96"/>
+        <v>232</v>
+      </c>
+      <c r="C106" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>Aimee</v>
+      </c>
+      <c r="D106" t="str" cm="1">
+        <f t="array" aca="1" ref="D106" ca="1">IF(_xlfn.XLOOKUP($B106,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B106,wordle_ids,wordles))</f>
+        <v>SKILL</v>
+      </c>
+      <c r="E106" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" s="2">
+        <f t="shared" ref="A107:B107" si="97">A100+1</f>
+        <v>44234</v>
+      </c>
+      <c r="B107" s="6">
+        <f t="shared" si="97"/>
+        <v>233</v>
+      </c>
+      <c r="C107" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>Phil</v>
+      </c>
+      <c r="D107" t="str" cm="1">
+        <f t="array" aca="1" ref="D107" ca="1">IF(_xlfn.XLOOKUP($B107,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B107,wordle_ids,wordles))</f>
+        <v>ELDER</v>
+      </c>
+      <c r="E107" s="10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="2">
+        <f t="shared" ref="A108:B108" si="98">A101+1</f>
+        <v>44234</v>
+      </c>
+      <c r="B108" s="6">
+        <f t="shared" si="98"/>
+        <v>233</v>
+      </c>
+      <c r="C108" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>Erik</v>
+      </c>
+      <c r="D108" t="str" cm="1">
+        <f t="array" aca="1" ref="D108" ca="1">IF(_xlfn.XLOOKUP($B108,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B108,wordle_ids,wordles))</f>
+        <v>ELDER</v>
+      </c>
+      <c r="E108" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" s="2">
+        <f t="shared" ref="A109:B109" si="99">A102+1</f>
+        <v>44234</v>
+      </c>
+      <c r="B109" s="6">
+        <f t="shared" si="99"/>
+        <v>233</v>
+      </c>
+      <c r="C109" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>RoBert</v>
+      </c>
+      <c r="D109" t="str" cm="1">
+        <f t="array" aca="1" ref="D109" ca="1">IF(_xlfn.XLOOKUP($B109,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B109,wordle_ids,wordles))</f>
+        <v>ELDER</v>
+      </c>
+      <c r="E109" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="2">
+        <f t="shared" ref="A110:B110" si="100">A103+1</f>
+        <v>44234</v>
+      </c>
+      <c r="B110" s="6">
+        <f t="shared" si="100"/>
+        <v>233</v>
+      </c>
+      <c r="C110" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>Andrew</v>
+      </c>
+      <c r="D110" t="str" cm="1">
+        <f t="array" aca="1" ref="D110" ca="1">IF(_xlfn.XLOOKUP($B110,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B110,wordle_ids,wordles))</f>
+        <v>ELDER</v>
+      </c>
+      <c r="E110" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="2">
+        <f t="shared" ref="A111:B111" si="101">A104+1</f>
+        <v>44234</v>
+      </c>
+      <c r="B111" s="6">
+        <f t="shared" si="101"/>
+        <v>233</v>
+      </c>
+      <c r="C111" s="2" t="str">
+        <f t="shared" ref="C111" si="102">C104</f>
+        <v>Yoyo</v>
+      </c>
+      <c r="D111" t="str" cm="1">
+        <f t="array" aca="1" ref="D111" ca="1">IF(_xlfn.XLOOKUP($B111,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B111,wordle_ids,wordles))</f>
+        <v>ELDER</v>
+      </c>
+      <c r="E111" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" s="2">
+        <f t="shared" ref="A112:B112" si="103">A105+1</f>
+        <v>44234</v>
+      </c>
+      <c r="B112" s="6">
+        <f t="shared" si="103"/>
+        <v>233</v>
+      </c>
+      <c r="C112" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>Henry</v>
+      </c>
+      <c r="D112" t="str" cm="1">
+        <f t="array" aca="1" ref="D112" ca="1">IF(_xlfn.XLOOKUP($B112,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B112,wordle_ids,wordles))</f>
+        <v>ELDER</v>
+      </c>
+      <c r="E112" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" s="2">
+        <f t="shared" ref="A113:B113" si="104">A106+1</f>
+        <v>44234</v>
+      </c>
+      <c r="B113" s="6">
+        <f t="shared" si="104"/>
+        <v>233</v>
+      </c>
+      <c r="C113" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>Aimee</v>
+      </c>
+      <c r="D113" t="str" cm="1">
+        <f t="array" aca="1" ref="D113" ca="1">IF(_xlfn.XLOOKUP($B113,wordle_ids,wordles)="","",_xlfn.XLOOKUP($B113,wordle_ids,wordles))</f>
+        <v>ELDER</v>
+      </c>
+      <c r="E113" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" s="2"/>
+      <c r="B114" s="6"/>
+      <c r="C114" s="2"/>
       <c r="E114" s="10"/>
     </row>
-    <row r="115" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" s="2"/>
+      <c r="B115" s="6"/>
+      <c r="C115" s="2"/>
       <c r="E115" s="10"/>
     </row>
-    <row r="116" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" s="2"/>
+      <c r="B116" s="6"/>
+      <c r="C116" s="2"/>
       <c r="E116" s="10"/>
     </row>
-    <row r="117" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E117" s="10"/>
     </row>
-    <row r="118" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E118" s="10"/>
     </row>
-    <row r="119" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E119" s="10"/>
     </row>
-    <row r="120" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E120" s="10"/>
     </row>
-    <row r="121" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E121" s="10"/>
     </row>
-    <row r="122" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E122" s="10"/>
     </row>
-    <row r="123" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E123" s="10"/>
     </row>
-    <row r="124" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E124" s="10"/>
     </row>
-    <row r="125" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E125" s="10"/>
     </row>
-    <row r="126" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E126" s="10"/>
     </row>
-    <row r="127" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E127" s="10"/>
     </row>
-    <row r="128" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E128" s="10"/>
     </row>
     <row r="129" spans="5:5" x14ac:dyDescent="0.25">
@@ -2874,19 +3259,64 @@
     <row r="242" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E242" s="10"/>
     </row>
+    <row r="243" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E243" s="10"/>
+    </row>
+    <row r="244" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E244" s="10"/>
+    </row>
+    <row r="245" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E245" s="10"/>
+    </row>
+    <row r="246" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E246" s="10"/>
+    </row>
+    <row r="247" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E247" s="10"/>
+    </row>
+    <row r="248" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E248" s="10"/>
+    </row>
+    <row r="249" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E249" s="10"/>
+    </row>
+    <row r="250" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E250" s="10"/>
+    </row>
+    <row r="251" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E251" s="10"/>
+    </row>
+    <row r="252" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E252" s="10"/>
+    </row>
+    <row r="253" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E253" s="10"/>
+    </row>
+    <row r="254" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E254" s="10"/>
+    </row>
+    <row r="255" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E255" s="10"/>
+    </row>
+    <row r="256" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E256" s="10"/>
+    </row>
+    <row r="257" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E257" s="10"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:E91" xr:uid="{2D001387-04E3-4955-8CAF-0DBBBF22CEAF}"/>
+  <autoFilter ref="A1:E113" xr:uid="{2D001387-04E3-4955-8CAF-0DBBBF22CEAF}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0627B16-E6A6-4FDA-A605-D8A29593EF93}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B36" sqref="B36"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2922,7 +3352,7 @@
         <v>44585</v>
       </c>
       <c r="B3" s="6">
-        <f t="shared" ref="B3:B16" si="0">B2+1</f>
+        <f t="shared" ref="B3:B17" si="0">B2+1</f>
         <v>219</v>
       </c>
       <c r="C3" s="9" t="s">
@@ -2931,7 +3361,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <f t="shared" ref="A4:A16" si="1">A3+1</f>
+        <f t="shared" ref="A4:A17" si="1">A3+1</f>
         <v>44586</v>
       </c>
       <c r="B4" s="6">
@@ -3098,6 +3528,19 @@
         <v>25</v>
       </c>
     </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <f t="shared" si="1"/>
+        <v>44599</v>
+      </c>
+      <c r="B17" s="6">
+        <f t="shared" si="0"/>
+        <v>233</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>